<commit_message>
Burning changes and minor error corrections in multiple files
</commit_message>
<xml_diff>
--- a/phpdocx/template/graph_excel.xlsx
+++ b/phpdocx/template/graph_excel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
   <si>
     <t>Shareholding Pattern</t>
   </si>
@@ -110,15 +110,15 @@
     <t>Non Audit</t>
   </si>
   <si>
-    <t>FY 11/12</t>
-  </si>
-  <si>
     <t>FY 12/13</t>
   </si>
   <si>
     <t>FY 13/14</t>
   </si>
   <si>
+    <t>FY 14/15</t>
+  </si>
+  <si>
     <t>Audit Fee</t>
   </si>
   <si>
@@ -137,13 +137,10 @@
     <t>Net Profit</t>
   </si>
   <si>
-    <t>FY 14/15</t>
-  </si>
-  <si>
-    <t>FY 10/11</t>
-  </si>
-  <si>
-    <t>FY 9/10</t>
+    <t>FY -1/le</t>
+  </si>
+  <si>
+    <t>FY -1/</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -164,15 +161,6 @@
     <t>Total Commission</t>
   </si>
   <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>S&amp;P CNX Nifty</t>
-  </si>
-  <si>
-    <t>CNX Finance</t>
-  </si>
-  <si>
     <t>Today</t>
   </si>
   <si>
@@ -194,10 +182,7 @@
     <t>Proposed increase</t>
   </si>
   <si>
-    <t>Mar'10</t>
-  </si>
-  <si>
-    <t>Sep'11</t>
+    <t>'</t>
   </si>
 </sst>
 </file>
@@ -991,16 +976,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>10</v>
+        <v>59.51</v>
       </c>
       <c r="D5" s="5">
-        <v>10</v>
+        <v>54.94</v>
       </c>
       <c r="E5" s="5">
-        <v>10</v>
+        <v>54.94</v>
       </c>
       <c r="F5" s="5">
-        <v>10</v>
+        <v>41.14</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1008,16 +993,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="5">
-        <v>37.96</v>
+        <v>1.37</v>
       </c>
       <c r="D6" s="5">
-        <v>42.1</v>
+        <v>2.49</v>
       </c>
       <c r="E6" s="5">
-        <v>40.52</v>
+        <v>2.49</v>
       </c>
       <c r="F6" s="5">
-        <v>39.02</v>
+        <v>2.49</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1025,16 +1010,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="5">
-        <v>15.1</v>
+        <v>1.96</v>
       </c>
       <c r="D7" s="5">
-        <v>-42.1</v>
+        <v>1.43</v>
       </c>
       <c r="E7" s="5">
-        <v>17.51</v>
+        <v>1.43</v>
       </c>
       <c r="F7" s="5">
-        <v>16.57</v>
+        <v>1.43</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1042,16 +1027,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="5">
-        <v>46.94</v>
+        <v>37.16</v>
       </c>
       <c r="D8" s="5">
-        <v>100</v>
+        <v>41.14</v>
       </c>
       <c r="E8" s="5">
-        <v>41.97</v>
+        <v>41.14</v>
       </c>
       <c r="F8" s="5">
-        <v>44.41</v>
+        <v>54.94</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1073,7 +1058,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1081,7 +1066,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="8">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1095,7 +1080,7 @@
         <v>10</v>
       </c>
       <c r="C28" s="10">
-        <v>0.8</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1103,7 +1088,7 @@
         <v>11</v>
       </c>
       <c r="C29" s="10">
-        <v>0.2</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1111,7 +1096,7 @@
         <v>12</v>
       </c>
       <c r="C30" s="10">
-        <v>0.2</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1119,7 +1104,7 @@
         <v>13</v>
       </c>
       <c r="C31" s="10">
-        <v>0.8</v>
+        <v>0.56</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1146,7 +1131,7 @@
         <v>0</v>
       </c>
       <c r="D38" s="15">
-        <v>125.66</v>
+        <v>62.2</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1157,7 +1142,7 @@
         <v>0</v>
       </c>
       <c r="D39" s="15">
-        <v>115.26</v>
+        <v>42.7</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1168,7 +1153,7 @@
         <v>0</v>
       </c>
       <c r="D40" s="15">
-        <v>119.33</v>
+        <v>34.55</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1176,10 +1161,10 @@
         <v>2014</v>
       </c>
       <c r="C41" s="21">
-        <v>0.83</v>
+        <v>0</v>
       </c>
       <c r="D41" s="15">
-        <v>138.61</v>
+        <v>42.07</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1187,10 +1172,10 @@
         <v>2015</v>
       </c>
       <c r="C42" s="22">
-        <v>6.08</v>
+        <v>14.12</v>
       </c>
       <c r="D42" s="17">
-        <v>186.28</v>
+        <v>43.26</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1212,7 +1197,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="19">
-        <v>0</v>
+        <v>0.14</v>
       </c>
       <c r="D50" s="20">
         <v>0</v>
@@ -1223,10 +1208,10 @@
         <v>21</v>
       </c>
       <c r="C51" s="19">
-        <v>0.11</v>
+        <v>0.19</v>
       </c>
       <c r="D51" s="20">
-        <v>0.07</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1246,13 +1231,13 @@
         <v>2013</v>
       </c>
       <c r="C60" s="43">
-        <v>42</v>
+        <v>0.1</v>
       </c>
       <c r="D60" s="44">
-        <v>158.76</v>
+        <v>1.39</v>
       </c>
       <c r="E60" s="45">
-        <v>30.75</v>
+        <v>8.36</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1260,13 +1245,13 @@
         <v>2014</v>
       </c>
       <c r="C61" s="43">
-        <v>63</v>
+        <v>3.25</v>
       </c>
       <c r="D61" s="44">
-        <v>178.39</v>
+        <v>3.67</v>
       </c>
       <c r="E61" s="45">
-        <v>41.05</v>
+        <v>102.93</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1274,13 +1259,13 @@
         <v>2015</v>
       </c>
       <c r="C62" s="43">
-        <v>59.5</v>
+        <v>4.1</v>
       </c>
       <c r="D62" s="44">
-        <v>105.91</v>
+        <v>6.5</v>
       </c>
       <c r="E62" s="45">
-        <v>65.3</v>
+        <v>73.31</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1296,44 +1281,44 @@
     </row>
     <row r="72" spans="1:6">
       <c r="B72" s="43">
-        <v>10</v>
+        <v>4.1</v>
       </c>
       <c r="C72" s="43">
-        <v>20</v>
+        <v>6.5</v>
       </c>
       <c r="D72" s="45">
-        <v>30</v>
+        <v>73.31</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="B73" s="43">
-        <v>40</v>
+        <v>20.7</v>
       </c>
       <c r="C73" s="43">
-        <v>50</v>
+        <v>21.19</v>
       </c>
       <c r="D73" s="45">
-        <v>60</v>
+        <v>113.54</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="B74" s="43">
-        <v>70</v>
+        <v>8.55</v>
       </c>
       <c r="C74" s="43">
-        <v>80</v>
+        <v>16.2</v>
       </c>
       <c r="D74" s="45">
-        <v>90</v>
+        <v>61.34</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="B82" s="23"/>
       <c r="C82" s="24">
+        <v>2015</v>
+      </c>
+      <c r="D82" s="24">
         <v>2014</v>
-      </c>
-      <c r="D82" s="24">
-        <v>2013</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -1341,10 +1326,10 @@
         <v>28</v>
       </c>
       <c r="C83" s="26">
-        <v>60</v>
+        <v>6.44</v>
       </c>
       <c r="D83" s="26">
-        <v>60</v>
+        <v>6.44</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -1352,10 +1337,10 @@
         <v>29</v>
       </c>
       <c r="C84" s="26">
-        <v>70</v>
+        <v>0.64</v>
       </c>
       <c r="D84" s="26">
-        <v>70</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -1363,10 +1348,10 @@
         <v>30</v>
       </c>
       <c r="C85" s="26">
-        <v>80</v>
+        <v>0.47</v>
       </c>
       <c r="D85" s="26">
-        <v>80</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="95" spans="1:6" customHeight="1" ht="15"/>
@@ -1387,13 +1372,13 @@
         <v>34</v>
       </c>
       <c r="C97" s="31">
-        <v>110</v>
+        <v>0.3</v>
       </c>
       <c r="D97" s="31">
-        <v>60</v>
+        <v>6.44</v>
       </c>
       <c r="E97" s="32">
-        <v>10</v>
+        <v>6.29</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -1401,13 +1386,13 @@
         <v>35</v>
       </c>
       <c r="C98" s="31">
-        <v>120</v>
+        <v>0.05</v>
       </c>
       <c r="D98" s="31">
-        <v>70</v>
+        <v>0.64</v>
       </c>
       <c r="E98" s="32">
-        <v>20</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="99" spans="1:6" customHeight="1" ht="15">
@@ -1415,13 +1400,13 @@
         <v>36</v>
       </c>
       <c r="C99" s="34">
-        <v>130</v>
+        <v>0.47</v>
       </c>
       <c r="D99" s="34">
-        <v>80</v>
+        <v>0.47</v>
       </c>
       <c r="E99" s="35">
-        <v>30</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="108" spans="1:6" customHeight="1" ht="15"/>
@@ -1441,275 +1426,187 @@
       <c r="B110" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="C110" s="31">
-        <v>6.08</v>
-      </c>
-      <c r="D110" s="31">
-        <v>186.28</v>
-      </c>
-      <c r="E110" s="32">
-        <v>12164</v>
-      </c>
+      <c r="C110" s="31"/>
+      <c r="D110" s="31"/>
+      <c r="E110" s="32"/>
     </row>
     <row r="111" spans="1:6">
       <c r="B111" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C111" s="31">
-        <v>0.83</v>
-      </c>
-      <c r="D111" s="31">
-        <v>138.61</v>
-      </c>
-      <c r="E111" s="32">
-        <v>10194</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C111" s="31"/>
+      <c r="D111" s="31"/>
+      <c r="E111" s="32"/>
     </row>
     <row r="112" spans="1:6">
       <c r="B112" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C112" s="31">
-        <v>0.9</v>
-      </c>
-      <c r="D112" s="31">
-        <v>119.33</v>
-      </c>
-      <c r="E112" s="32">
-        <v>9116</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C112" s="31"/>
+      <c r="D112" s="31"/>
+      <c r="E112" s="32"/>
     </row>
     <row r="113" spans="1:6">
       <c r="B113" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C113" s="31">
-        <v>0.89</v>
-      </c>
-      <c r="D113" s="31">
-        <v>115.26</v>
-      </c>
-      <c r="E113" s="32">
-        <v>8470</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C113" s="31"/>
+      <c r="D113" s="31"/>
+      <c r="E113" s="32"/>
     </row>
     <row r="114" spans="1:6" customHeight="1" ht="15">
       <c r="B114" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="C114" s="34">
-        <v>0.87</v>
-      </c>
-      <c r="D114" s="34">
-        <v>125.66</v>
-      </c>
-      <c r="E114" s="32">
-        <v>6443</v>
-      </c>
+      <c r="C114" s="34"/>
+      <c r="D114" s="34"/>
+      <c r="E114" s="32"/>
     </row>
     <row r="115" spans="1:6" customHeight="1" ht="15">
       <c r="B115" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="C115" s="34">
-        <v>0.65</v>
-      </c>
-      <c r="D115" s="34">
-        <v>125.66</v>
-      </c>
-      <c r="E115" s="35">
-        <v>6443</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C115" s="34"/>
+      <c r="D115" s="34"/>
+      <c r="E115" s="35"/>
     </row>
     <row r="122" spans="1:6">
       <c r="C122" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D122" s="31" t="s">
         <v>43</v>
-      </c>
-      <c r="D122" s="31" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="C123" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D123" s="36">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:6">
       <c r="C124" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D124" s="36">
-        <v>20</v>
+        <v>8.2</v>
       </c>
     </row>
     <row r="125" spans="1:6">
       <c r="C125" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D125" s="36">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D133" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="C134" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="D134" s="36">
-        <v>17.89</v>
-      </c>
+      <c r="D134" s="36"/>
     </row>
     <row r="135" spans="1:6">
       <c r="C135" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="D135" s="36">
-        <v>40.11</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D135" s="36"/>
     </row>
     <row r="136" spans="1:6">
       <c r="C136" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="D136" s="36">
-        <v>50.44</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D136" s="36"/>
     </row>
     <row r="137" spans="1:6">
       <c r="C137" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D137" s="36">
-        <v>63.61</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D137" s="36"/>
     </row>
     <row r="138" spans="1:6">
       <c r="C138" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="D138" s="36">
-        <v>128.83</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="D138" s="36"/>
     </row>
     <row r="153" spans="1:6">
       <c r="B153" s="31"/>
-      <c r="C153" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="D153" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="E153" s="31" t="s">
-        <v>51</v>
-      </c>
+      <c r="C153" s="31"/>
+      <c r="D153" s="31"/>
+      <c r="E153" s="31"/>
     </row>
     <row r="154" spans="1:6">
       <c r="B154" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="C154" s="31">
-        <v>90</v>
-      </c>
-      <c r="D154" s="31">
-        <v>9</v>
-      </c>
-      <c r="E154" s="31">
-        <v>9</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C154" s="31"/>
+      <c r="D154" s="31"/>
+      <c r="E154" s="31"/>
     </row>
     <row r="155" spans="1:6">
       <c r="B155" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="C155" s="31">
-        <v>9</v>
-      </c>
-      <c r="D155" s="31">
-        <v>9</v>
-      </c>
-      <c r="E155" s="31">
-        <v>9</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C155" s="31"/>
+      <c r="D155" s="31"/>
+      <c r="E155" s="31"/>
     </row>
     <row r="156" spans="1:6">
       <c r="B156" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="C156" s="31">
-        <v>9</v>
-      </c>
-      <c r="D156" s="31">
-        <v>0</v>
-      </c>
-      <c r="E156" s="31">
-        <v>90</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C156" s="31"/>
+      <c r="D156" s="31"/>
+      <c r="E156" s="31"/>
     </row>
     <row r="157" spans="1:6">
       <c r="B157" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C157" s="31">
-        <v>90</v>
-      </c>
-      <c r="D157" s="31">
-        <v>90</v>
-      </c>
-      <c r="E157" s="31">
-        <v>9</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C157" s="31"/>
+      <c r="D157" s="31"/>
+      <c r="E157" s="31"/>
     </row>
     <row r="483" spans="1:6" customHeight="1" ht="28">
       <c r="B483" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C483" s="39" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D483" s="39" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E483" s="39" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="484" spans="1:6">
       <c r="B484" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="C484" s="40">
-        <v>30</v>
-      </c>
-      <c r="D484" s="40">
-        <v>40</v>
-      </c>
-      <c r="E484" s="40">
-        <v>50</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C484" s="40"/>
+      <c r="D484" s="40"/>
+      <c r="E484" s="40"/>
     </row>
     <row r="485" spans="1:6">
       <c r="B485" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="C485" s="40">
-        <v>90</v>
-      </c>
-      <c r="D485" s="40">
-        <v>90</v>
-      </c>
-      <c r="E485" s="40">
-        <v>90</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C485" s="40"/>
+      <c r="D485" s="40"/>
+      <c r="E485" s="40"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Burning and Database file changes
</commit_message>
<xml_diff>
--- a/phpdocx/template/graph_excel.xlsx
+++ b/phpdocx/template/graph_excel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
   <si>
     <t>Shareholding Pattern</t>
   </si>
@@ -74,6 +74,9 @@
     <t>Non-Executive</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>Non-Promoter</t>
   </si>
   <si>
@@ -104,7 +107,13 @@
     <t>Non Audit</t>
   </si>
   <si>
-    <t>FY -1/0</t>
+    <t>FY 12/13</t>
+  </si>
+  <si>
+    <t>FY 13/14</t>
+  </si>
+  <si>
+    <t>FY 14/15</t>
   </si>
   <si>
     <t>Audit Fee</t>
@@ -125,7 +134,13 @@
     <t>Net Profit</t>
   </si>
   <si>
-    <t>FY -1/</t>
+    <t>FY 11/12</t>
+  </si>
+  <si>
+    <t>FY 10/11</t>
+  </si>
+  <si>
+    <t>FY 9/10</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -195,15 +210,6 @@
   </si>
   <si>
     <t>CSR as % of Net Profit</t>
-  </si>
-  <si>
-    <t>FY 12/13</t>
-  </si>
-  <si>
-    <t>FY 13/14</t>
-  </si>
-  <si>
-    <t>FY 14/15</t>
   </si>
   <si>
     <t>d</t>
@@ -1010,46 +1016,86 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="C4" s="3">
+        <v>2015</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2014</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2013</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2012</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="C5" s="5">
+        <v>59.51</v>
+      </c>
+      <c r="D5" s="5">
+        <v>54.94</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="C6" s="5">
+        <v>1.37</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2.49</v>
+      </c>
+      <c r="E6" s="5">
+        <v>27.23</v>
+      </c>
+      <c r="F6" s="5">
+        <v>24.97</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="C7" s="5">
+        <v>1.96</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1.43</v>
+      </c>
+      <c r="E7" s="5">
+        <v>4.24</v>
+      </c>
+      <c r="F7" s="5">
+        <v>4.76</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="C8" s="5">
+        <v>37.16</v>
+      </c>
+      <c r="D8" s="5">
+        <v>41.14</v>
+      </c>
+      <c r="E8" s="5">
+        <v>68.53</v>
+      </c>
+      <c r="F8" s="5">
+        <v>70.27</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="6" t="s">
@@ -1061,19 +1107,25 @@
       <c r="B16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="8"/>
+      <c r="C16" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="B17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" s="46"/>
@@ -1089,30 +1141,30 @@
         <v>10</v>
       </c>
       <c r="C28" s="49">
-        <v>0</v>
-      </c>
-      <c r="D28" s="49"/>
+        <v>0.38</v>
+      </c>
+      <c r="D28" s="49">
+        <v>0.63</v>
+      </c>
     </row>
     <row r="29" spans="1:6">
       <c r="B29" s="48" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="49">
-        <v>0</v>
-      </c>
-      <c r="D29" s="49"/>
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="49">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="30" spans="1:6">
       <c r="B30" s="44"/>
-      <c r="C30" s="45">
-        <v>0</v>
-      </c>
+      <c r="C30" s="45"/>
     </row>
     <row r="31" spans="1:6">
       <c r="B31" s="44"/>
-      <c r="C31" s="45">
-        <v>0</v>
-      </c>
+      <c r="C31" s="45"/>
     </row>
     <row r="36" spans="1:6">
       <c r="B36" t="s">
@@ -1131,29 +1183,59 @@
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="B38" s="12"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="13"/>
+      <c r="B38" s="12">
+        <v>2011</v>
+      </c>
+      <c r="C38" s="19">
+        <v>0</v>
+      </c>
+      <c r="D38" s="13">
+        <v>62.89</v>
+      </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="B39" s="12"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="13"/>
+      <c r="B39" s="12">
+        <v>2012</v>
+      </c>
+      <c r="C39" s="19">
+        <v>0</v>
+      </c>
+      <c r="D39" s="13">
+        <v>43.39</v>
+      </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="B40" s="12"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="13"/>
+      <c r="B40" s="12">
+        <v>2013</v>
+      </c>
+      <c r="C40" s="19">
+        <v>0</v>
+      </c>
+      <c r="D40" s="13">
+        <v>35.24</v>
+      </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="B41" s="12"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="13"/>
+      <c r="B41" s="12">
+        <v>2014</v>
+      </c>
+      <c r="C41" s="19">
+        <v>6.25</v>
+      </c>
+      <c r="D41" s="13">
+        <v>42.76</v>
+      </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="B42" s="14"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="15"/>
+      <c r="B42" s="14">
+        <v>2015</v>
+      </c>
+      <c r="C42" s="20">
+        <v>14.12</v>
+      </c>
+      <c r="D42" s="15">
+        <v>43.95</v>
+      </c>
     </row>
     <row r="48" spans="1:6">
       <c r="B48" t="s">
@@ -1173,55 +1255,87 @@
       <c r="B50" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="18"/>
+      <c r="C50" s="17">
+        <v>14.12</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="51" spans="1:6">
       <c r="B51" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="18"/>
+        <v>20</v>
+      </c>
+      <c r="C51" s="17">
+        <v>6.32</v>
+      </c>
+      <c r="D51" s="18">
+        <v>0.45</v>
+      </c>
     </row>
     <row r="59" spans="1:6">
       <c r="B59" s="39"/>
       <c r="C59" s="40" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D59" s="40" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E59" s="40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="B60" s="40"/>
-      <c r="C60" s="41"/>
-      <c r="D60" s="42"/>
-      <c r="E60" s="43"/>
+      <c r="B60" s="40">
+        <v>2013</v>
+      </c>
+      <c r="C60" s="41">
+        <v>0.1</v>
+      </c>
+      <c r="D60" s="42">
+        <v>1.39</v>
+      </c>
+      <c r="E60" s="43">
+        <v>8.36</v>
+      </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="B61" s="40"/>
-      <c r="C61" s="41"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="43"/>
+      <c r="B61" s="40">
+        <v>2014</v>
+      </c>
+      <c r="C61" s="41">
+        <v>3.25</v>
+      </c>
+      <c r="D61" s="42">
+        <v>3.67</v>
+      </c>
+      <c r="E61" s="43">
+        <v>102.93</v>
+      </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="B62" s="40"/>
-      <c r="C62" s="41"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="43"/>
+      <c r="B62" s="40">
+        <v>2015</v>
+      </c>
+      <c r="C62" s="41">
+        <v>4.1</v>
+      </c>
+      <c r="D62" s="42">
+        <v>6.5</v>
+      </c>
+      <c r="E62" s="43">
+        <v>73.31</v>
+      </c>
     </row>
     <row r="71" spans="1:6">
       <c r="B71" s="40" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C71" s="40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D71" s="40" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1241,191 +1355,277 @@
     </row>
     <row r="82" spans="1:6">
       <c r="B82" s="21"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="22"/>
+      <c r="C82" s="22">
+        <v>2015</v>
+      </c>
+      <c r="D82" s="22">
+        <v>2014</v>
+      </c>
     </row>
     <row r="83" spans="1:6">
       <c r="B83" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C83" s="24"/>
-      <c r="D83" s="24"/>
+        <v>27</v>
+      </c>
+      <c r="C83" s="24">
+        <v>0.84</v>
+      </c>
+      <c r="D83" s="24">
+        <v>0.84</v>
+      </c>
     </row>
     <row r="84" spans="1:6">
       <c r="B84" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
+        <v>28</v>
+      </c>
+      <c r="C84" s="24">
+        <v>0.64</v>
+      </c>
+      <c r="D84" s="24">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="85" spans="1:6">
       <c r="B85" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
+        <v>29</v>
+      </c>
+      <c r="C85" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="D85" s="24">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="95" spans="1:6" customHeight="1" ht="15"/>
     <row r="96" spans="1:6">
       <c r="B96" s="25"/>
       <c r="C96" s="26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E96" s="27" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="B97" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C97" s="29"/>
-      <c r="D97" s="29"/>
-      <c r="E97" s="30"/>
+        <v>33</v>
+      </c>
+      <c r="C97" s="29">
+        <v>0.47</v>
+      </c>
+      <c r="D97" s="29">
+        <v>0.84</v>
+      </c>
+      <c r="E97" s="30">
+        <v>6.29</v>
+      </c>
     </row>
     <row r="98" spans="1:6">
       <c r="B98" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C98" s="29"/>
-      <c r="D98" s="29"/>
-      <c r="E98" s="30"/>
+        <v>34</v>
+      </c>
+      <c r="C98" s="29">
+        <v>0.14</v>
+      </c>
+      <c r="D98" s="29">
+        <v>0.64</v>
+      </c>
+      <c r="E98" s="30">
+        <v>6.44</v>
+      </c>
     </row>
     <row r="99" spans="1:6" customHeight="1" ht="15">
       <c r="B99" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C99" s="32"/>
-      <c r="D99" s="32"/>
-      <c r="E99" s="33"/>
+        <v>35</v>
+      </c>
+      <c r="C99" s="32">
+        <v>2.11</v>
+      </c>
+      <c r="D99" s="32">
+        <v>0.05</v>
+      </c>
+      <c r="E99" s="33">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="108" spans="1:6" customHeight="1" ht="15"/>
     <row r="109" spans="1:6">
       <c r="B109" s="25"/>
       <c r="C109" s="26" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D109" s="26" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E109" s="27" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="B110" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C110" s="29"/>
-      <c r="D110" s="29"/>
-      <c r="E110" s="30"/>
+        <v>32</v>
+      </c>
+      <c r="C110" s="29">
+        <v>14.12</v>
+      </c>
+      <c r="D110" s="29">
+        <v>43.95</v>
+      </c>
+      <c r="E110" s="30">
+        <v>1927.2</v>
+      </c>
     </row>
     <row r="111" spans="1:6">
       <c r="B111" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C111" s="29"/>
-      <c r="D111" s="29"/>
-      <c r="E111" s="30"/>
+        <v>31</v>
+      </c>
+      <c r="C111" s="29">
+        <v>6.25</v>
+      </c>
+      <c r="D111" s="29">
+        <v>42.76</v>
+      </c>
+      <c r="E111" s="30">
+        <v>1076.09</v>
+      </c>
     </row>
     <row r="112" spans="1:6">
       <c r="B112" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C112" s="29"/>
-      <c r="D112" s="29"/>
-      <c r="E112" s="30"/>
+        <v>30</v>
+      </c>
+      <c r="C112" s="29">
+        <v>0</v>
+      </c>
+      <c r="D112" s="29">
+        <v>35.24</v>
+      </c>
+      <c r="E112" s="30">
+        <v>120.77</v>
+      </c>
     </row>
     <row r="113" spans="1:6">
       <c r="B113" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C113" s="29"/>
-      <c r="D113" s="29"/>
-      <c r="E113" s="30"/>
+        <v>39</v>
+      </c>
+      <c r="C113" s="29">
+        <v>0</v>
+      </c>
+      <c r="D113" s="29">
+        <v>43.39</v>
+      </c>
+      <c r="E113" s="30">
+        <v>1679.94</v>
+      </c>
     </row>
     <row r="114" spans="1:6" customHeight="1" ht="15">
       <c r="B114" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C114" s="32"/>
-      <c r="D114" s="32"/>
-      <c r="E114" s="30"/>
+        <v>40</v>
+      </c>
+      <c r="C114" s="32">
+        <v>0</v>
+      </c>
+      <c r="D114" s="32">
+        <v>62.89</v>
+      </c>
+      <c r="E114" s="30">
+        <v>3432.8</v>
+      </c>
     </row>
     <row r="115" spans="1:6" customHeight="1" ht="15">
       <c r="B115" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C115" s="32"/>
-      <c r="D115" s="32"/>
-      <c r="E115" s="33"/>
+        <v>41</v>
+      </c>
+      <c r="C115" s="32">
+        <v>0</v>
+      </c>
+      <c r="D115" s="32">
+        <v>47435</v>
+      </c>
+      <c r="E115" s="33">
+        <v>2188.09</v>
+      </c>
     </row>
     <row r="122" spans="1:6">
       <c r="C122" s="29" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D122" s="29" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="C123" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D123" s="34"/>
+        <v>44</v>
+      </c>
+      <c r="D123" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="1:6">
       <c r="C124" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D124" s="34"/>
+        <v>45</v>
+      </c>
+      <c r="D124" s="34">
+        <v>41.25</v>
+      </c>
     </row>
     <row r="125" spans="1:6">
       <c r="C125" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D125" s="34"/>
+        <v>46</v>
+      </c>
+      <c r="D125" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="29" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="C134" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D134" s="34"/>
+        <v>40</v>
+      </c>
+      <c r="D134" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="135" spans="1:6">
       <c r="C135" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D135" s="34"/>
+        <v>39</v>
+      </c>
+      <c r="D135" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="136" spans="1:6">
       <c r="C136" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D136" s="34"/>
+        <v>30</v>
+      </c>
+      <c r="D136" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="137" spans="1:6">
       <c r="C137" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D137" s="34"/>
+        <v>31</v>
+      </c>
+      <c r="D137" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="138" spans="1:6">
       <c r="C138" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D138" s="34"/>
+        <v>32</v>
+      </c>
+      <c r="D138" s="34">
+        <v>41.25</v>
+      </c>
     </row>
     <row r="153" spans="1:6">
       <c r="B153" s="29"/>
@@ -1433,99 +1633,99 @@
         <v>11</v>
       </c>
       <c r="D153" s="29" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E153" s="29" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="154" spans="1:6">
       <c r="B154" s="35" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C154" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D154" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E154" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="155" spans="1:6">
       <c r="B155" s="35" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C155" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D155" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E155" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="156" spans="1:6">
       <c r="B156" s="35" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C156" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D156" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E156" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="157" spans="1:6">
       <c r="B157" s="35" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C157" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D157" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E157" s="29" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="483" spans="1:6" customHeight="1" ht="28">
       <c r="B483" s="36" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C483" s="37" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D483" s="37" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E483" s="37" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="484" spans="1:6">
       <c r="B484" s="29" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C484" s="38" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D484" s="38" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E484" s="38" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
     <row r="485" spans="1:6">
       <c r="B485" s="29" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C485" s="38"/>
       <c r="D485" s="38"/>
@@ -1533,7 +1733,7 @@
     </row>
     <row r="493" spans="1:6">
       <c r="C493" s="51" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D493" s="52">
         <v>123</v>
@@ -1543,7 +1743,7 @@
     </row>
     <row r="494" spans="1:6">
       <c r="C494" s="51" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D494" s="52">
         <v>187</v>
@@ -1553,7 +1753,7 @@
     </row>
     <row r="495" spans="1:6">
       <c r="C495" s="51" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D495" s="52">
         <v>115</v>
@@ -1563,7 +1763,7 @@
     </row>
     <row r="496" spans="1:6">
       <c r="C496" s="51" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D496" s="52">
         <v>10</v>
@@ -1615,7 +1815,7 @@
     </row>
     <row r="504" spans="1:6">
       <c r="C504" s="51" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D504" s="52"/>
       <c r="E504" s="50"/>
@@ -1623,7 +1823,7 @@
     </row>
     <row r="505" spans="1:6">
       <c r="C505" s="51" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D505" s="52"/>
       <c r="E505" s="50"/>
@@ -1631,7 +1831,7 @@
     </row>
     <row r="506" spans="1:6">
       <c r="C506" s="51" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D506" s="52"/>
       <c r="E506" s="50"/>
@@ -1639,7 +1839,7 @@
     </row>
     <row r="507" spans="1:6">
       <c r="C507" s="51" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D507" s="52"/>
       <c r="E507" s="50"/>
@@ -1689,19 +1889,19 @@
     </row>
     <row r="515" spans="1:6">
       <c r="C515" s="29" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D515" s="29" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="E515" s="29" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F515" s="50"/>
     </row>
     <row r="516" spans="1:6">
       <c r="C516" s="29" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D516" s="53">
         <v>26168</v>
@@ -1713,7 +1913,7 @@
     </row>
     <row r="517" spans="1:6">
       <c r="C517" s="29" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="D517" s="53">
         <v>268</v>
@@ -1725,10 +1925,10 @@
     </row>
     <row r="518" spans="1:6">
       <c r="C518" s="29" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="D518" s="53" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E518" s="54">
         <v>167</v>

</xml_diff>

<commit_message>
Burning and input sheet changes
</commit_message>
<xml_diff>
--- a/phpdocx/template/graph_excel.xlsx
+++ b/phpdocx/template/graph_excel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>Shareholding Pattern</t>
   </si>
@@ -134,13 +134,7 @@
     <t>Net Profit</t>
   </si>
   <si>
-    <t>FY 11/12</t>
-  </si>
-  <si>
-    <t>FY 10/11</t>
-  </si>
-  <si>
-    <t>FY 9/10</t>
+    <t>FY -1/</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -161,15 +155,6 @@
     <t>Total Commission</t>
   </si>
   <si>
-    <t>Vedanta</t>
-  </si>
-  <si>
-    <t>S&amp;P CNX Nifty</t>
-  </si>
-  <si>
-    <t>CNX Finance</t>
-  </si>
-  <si>
     <t>Today</t>
   </si>
   <si>
@@ -191,22 +176,16 @@
     <t>Proposed increase</t>
   </si>
   <si>
-    <t>Mar'15</t>
-  </si>
-  <si>
-    <t>Mar'14</t>
-  </si>
-  <si>
-    <t>Mar'13</t>
-  </si>
-  <si>
-    <t>Mar'12</t>
+    <t>'</t>
   </si>
   <si>
     <t>CSR</t>
   </si>
   <si>
     <t>CSR as % of Net Profit</t>
+  </si>
+  <si>
+    <t>FY -1/0</t>
   </si>
 </sst>
 </file>
@@ -1028,16 +1007,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>59.51</v>
+        <v>73.39</v>
       </c>
       <c r="D5" s="5">
-        <v>54.94</v>
+        <v>73.47</v>
       </c>
       <c r="E5" s="5">
-        <v>30</v>
+        <v>78.28</v>
       </c>
       <c r="F5" s="5">
-        <v>37.7</v>
+        <v>78.41</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1045,16 +1024,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="5">
-        <v>1.37</v>
+        <v>10.71</v>
       </c>
       <c r="D6" s="5">
-        <v>2.49</v>
+        <v>10.13</v>
       </c>
       <c r="E6" s="5">
-        <v>27.23</v>
+        <v>7.3</v>
       </c>
       <c r="F6" s="5">
-        <v>24.97</v>
+        <v>6.67</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1062,16 +1041,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="5">
-        <v>1.96</v>
+        <v>4.36</v>
       </c>
       <c r="D7" s="5">
-        <v>1.43</v>
+        <v>3.49</v>
       </c>
       <c r="E7" s="5">
-        <v>4.24</v>
+        <v>3.32</v>
       </c>
       <c r="F7" s="5">
-        <v>4.76</v>
+        <v>3.41</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1079,16 +1058,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="5">
-        <v>37.16</v>
+        <v>11.54</v>
       </c>
       <c r="D8" s="5">
-        <v>41.14</v>
+        <v>12.91</v>
       </c>
       <c r="E8" s="5">
-        <v>38.53</v>
+        <v>11.1</v>
       </c>
       <c r="F8" s="5">
-        <v>32.57</v>
+        <v>11.51</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1110,7 +1089,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="8">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1118,7 +1097,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="8">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1135,10 +1114,10 @@
         <v>10</v>
       </c>
       <c r="C28" s="49">
-        <v>0.38</v>
+        <v>0.4</v>
       </c>
       <c r="D28" s="49">
-        <v>0.63</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1146,10 +1125,10 @@
         <v>11</v>
       </c>
       <c r="C29" s="49">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="D29" s="49">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1181,10 +1160,10 @@
         <v>2011</v>
       </c>
       <c r="C38" s="19">
-        <v>0</v>
+        <v>1.12</v>
       </c>
       <c r="D38" s="13">
-        <v>62.89</v>
+        <v>113.96</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1192,10 +1171,10 @@
         <v>2012</v>
       </c>
       <c r="C39" s="19">
-        <v>0</v>
+        <v>1.97</v>
       </c>
       <c r="D39" s="13">
-        <v>43.39</v>
+        <v>106.12</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1203,10 +1182,10 @@
         <v>2013</v>
       </c>
       <c r="C40" s="19">
-        <v>0</v>
+        <v>3.39</v>
       </c>
       <c r="D40" s="13">
-        <v>35.24</v>
+        <v>107.33</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1214,10 +1193,10 @@
         <v>2014</v>
       </c>
       <c r="C41" s="19">
-        <v>6.25</v>
+        <v>10.24</v>
       </c>
       <c r="D41" s="13">
-        <v>42.76</v>
+        <v>134.55</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1225,10 +1204,10 @@
         <v>2015</v>
       </c>
       <c r="C42" s="20">
-        <v>14.12</v>
+        <v>4.77</v>
       </c>
       <c r="D42" s="15">
-        <v>43.95</v>
+        <v>156.9</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1250,7 +1229,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="17">
-        <v>14.12</v>
+        <v>3.73</v>
       </c>
       <c r="D50" s="18" t="s">
         <v>19</v>
@@ -1261,10 +1240,10 @@
         <v>20</v>
       </c>
       <c r="C51" s="17">
-        <v>6.32</v>
+        <v>8.94</v>
       </c>
       <c r="D51" s="18">
-        <v>0.45</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1284,13 +1263,13 @@
         <v>2013</v>
       </c>
       <c r="C60" s="41">
-        <v>0.1</v>
+        <v>7</v>
       </c>
       <c r="D60" s="42">
-        <v>1.39</v>
+        <v>23.03</v>
       </c>
       <c r="E60" s="43">
-        <v>8.36</v>
+        <v>35.33</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1298,13 +1277,13 @@
         <v>2014</v>
       </c>
       <c r="C61" s="41">
-        <v>3.25</v>
+        <v>8</v>
       </c>
       <c r="D61" s="42">
-        <v>3.67</v>
+        <v>30.09</v>
       </c>
       <c r="E61" s="43">
-        <v>102.93</v>
+        <v>30.9</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1312,13 +1291,13 @@
         <v>2015</v>
       </c>
       <c r="C62" s="41">
-        <v>4.1</v>
+        <v>12</v>
       </c>
       <c r="D62" s="42">
-        <v>6.5</v>
+        <v>33.38</v>
       </c>
       <c r="E62" s="43">
-        <v>73.31</v>
+        <v>41.78</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1334,35 +1313,35 @@
     </row>
     <row r="72" spans="1:6">
       <c r="B72" s="41">
-        <v>4.1</v>
+        <v>12</v>
       </c>
       <c r="C72" s="41">
-        <v>6.5</v>
+        <v>33.38</v>
       </c>
       <c r="D72" s="43">
-        <v>73.31</v>
+        <v>41.78</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="B73" s="41">
-        <v>20.7</v>
+        <v>59.5</v>
       </c>
       <c r="C73" s="41">
-        <v>21.19</v>
+        <v>105.91</v>
       </c>
       <c r="D73" s="43">
-        <v>113.54</v>
+        <v>65.3</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="B74" s="41">
-        <v>8.55</v>
+        <v>79</v>
       </c>
       <c r="C74" s="41">
-        <v>16.2</v>
+        <v>98.31</v>
       </c>
       <c r="D74" s="43">
-        <v>61.34</v>
+        <v>93.4</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -1379,10 +1358,10 @@
         <v>27</v>
       </c>
       <c r="C83" s="24">
-        <v>6.44</v>
+        <v>4.4</v>
       </c>
       <c r="D83" s="24">
-        <v>6.44</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -1390,10 +1369,10 @@
         <v>28</v>
       </c>
       <c r="C84" s="24">
-        <v>0.64</v>
+        <v>0.4</v>
       </c>
       <c r="D84" s="24">
-        <v>0.64</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -1401,10 +1380,10 @@
         <v>29</v>
       </c>
       <c r="C85" s="24">
-        <v>0.14</v>
+        <v>0</v>
       </c>
       <c r="D85" s="24">
-        <v>0.14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:6" customHeight="1" ht="15"/>
@@ -1425,13 +1404,13 @@
         <v>33</v>
       </c>
       <c r="C97" s="29">
-        <v>0.3</v>
+        <v>4.3</v>
       </c>
       <c r="D97" s="29">
-        <v>6.44</v>
+        <v>4.4</v>
       </c>
       <c r="E97" s="30">
-        <v>6.29</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -1439,13 +1418,13 @@
         <v>34</v>
       </c>
       <c r="C98" s="29">
-        <v>0.05</v>
+        <v>0.4</v>
       </c>
       <c r="D98" s="29">
-        <v>0.64</v>
+        <v>0.4</v>
       </c>
       <c r="E98" s="30">
-        <v>0.84</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="99" spans="1:6" customHeight="1" ht="15">
@@ -1453,13 +1432,13 @@
         <v>35</v>
       </c>
       <c r="C99" s="32">
-        <v>2.11</v>
+        <v>0</v>
       </c>
       <c r="D99" s="32">
-        <v>0.14</v>
+        <v>0</v>
       </c>
       <c r="E99" s="33">
-        <v>0.47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:6" customHeight="1" ht="15"/>
@@ -1477,313 +1456,213 @@
     </row>
     <row r="110" spans="1:6">
       <c r="B110" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C110" s="29">
-        <v>14.12</v>
-      </c>
-      <c r="D110" s="29">
-        <v>43.95</v>
-      </c>
-      <c r="E110" s="30">
-        <v>1927.2</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C110" s="29"/>
+      <c r="D110" s="29"/>
+      <c r="E110" s="30"/>
     </row>
     <row r="111" spans="1:6">
       <c r="B111" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C111" s="29">
-        <v>6.25</v>
-      </c>
-      <c r="D111" s="29">
-        <v>42.76</v>
-      </c>
-      <c r="E111" s="30">
-        <v>1076.09</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C111" s="29"/>
+      <c r="D111" s="29"/>
+      <c r="E111" s="30"/>
     </row>
     <row r="112" spans="1:6">
       <c r="B112" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C112" s="29">
-        <v>0</v>
-      </c>
-      <c r="D112" s="29">
-        <v>35.24</v>
-      </c>
-      <c r="E112" s="30">
-        <v>120.77</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C112" s="29"/>
+      <c r="D112" s="29"/>
+      <c r="E112" s="30"/>
     </row>
     <row r="113" spans="1:6">
       <c r="B113" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C113" s="29">
-        <v>0</v>
-      </c>
-      <c r="D113" s="29">
-        <v>43.39</v>
-      </c>
-      <c r="E113" s="30">
-        <v>1679.94</v>
-      </c>
+      <c r="C113" s="29"/>
+      <c r="D113" s="29"/>
+      <c r="E113" s="30"/>
     </row>
     <row r="114" spans="1:6" customHeight="1" ht="15">
       <c r="B114" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="C114" s="32">
-        <v>0</v>
-      </c>
-      <c r="D114" s="32">
-        <v>62.89</v>
-      </c>
-      <c r="E114" s="30">
-        <v>3432.8</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C114" s="32"/>
+      <c r="D114" s="32"/>
+      <c r="E114" s="30"/>
     </row>
     <row r="115" spans="1:6" customHeight="1" ht="15">
       <c r="B115" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="C115" s="32">
-        <v>0</v>
-      </c>
-      <c r="D115" s="32">
-        <v>47435</v>
-      </c>
-      <c r="E115" s="33">
-        <v>2188.09</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C115" s="32"/>
+      <c r="D115" s="32"/>
+      <c r="E115" s="33"/>
     </row>
     <row r="122" spans="1:6">
       <c r="C122" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D122" s="29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="C123" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="D123" s="34">
-        <v>0</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D123" s="34"/>
     </row>
     <row r="124" spans="1:6">
       <c r="C124" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D124" s="34">
-        <v>41.25</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D124" s="34"/>
     </row>
     <row r="125" spans="1:6">
       <c r="C125" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D125" s="34">
-        <v>0</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D125" s="34"/>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="C134" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D134" s="34">
-        <v>0</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D134" s="34"/>
     </row>
     <row r="135" spans="1:6">
       <c r="C135" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D135" s="34">
-        <v>0</v>
-      </c>
+      <c r="D135" s="34"/>
     </row>
     <row r="136" spans="1:6">
       <c r="C136" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="D136" s="34">
-        <v>0</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D136" s="34"/>
     </row>
     <row r="137" spans="1:6">
       <c r="C137" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D137" s="34">
-        <v>0</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D137" s="34"/>
     </row>
     <row r="138" spans="1:6">
       <c r="C138" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D138" s="34">
-        <v>41.25</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D138" s="34"/>
     </row>
     <row r="153" spans="1:6">
       <c r="B153" s="29"/>
-      <c r="C153" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D153" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="E153" s="29" t="s">
-        <v>50</v>
-      </c>
+      <c r="C153" s="29"/>
+      <c r="D153" s="29"/>
+      <c r="E153" s="29"/>
     </row>
     <row r="154" spans="1:6">
       <c r="B154" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="C154" s="29">
-        <v>112</v>
-      </c>
-      <c r="D154" s="29">
-        <v>100</v>
-      </c>
-      <c r="E154" s="29">
-        <v>198</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C154" s="29"/>
+      <c r="D154" s="29"/>
+      <c r="E154" s="29"/>
     </row>
     <row r="155" spans="1:6">
       <c r="B155" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="C155" s="29">
-        <v>110</v>
-      </c>
-      <c r="D155" s="29">
-        <v>90</v>
-      </c>
-      <c r="E155" s="29">
-        <v>195</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C155" s="29"/>
+      <c r="D155" s="29"/>
+      <c r="E155" s="29"/>
     </row>
     <row r="156" spans="1:6">
       <c r="B156" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="C156" s="29">
-        <v>105</v>
-      </c>
-      <c r="D156" s="29">
-        <v>85</v>
-      </c>
-      <c r="E156" s="29">
-        <v>185</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C156" s="29"/>
+      <c r="D156" s="29"/>
+      <c r="E156" s="29"/>
     </row>
     <row r="157" spans="1:6">
       <c r="B157" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C157" s="29">
-        <v>100</v>
-      </c>
-      <c r="D157" s="29">
-        <v>75</v>
-      </c>
-      <c r="E157" s="29">
-        <v>175</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C157" s="29"/>
+      <c r="D157" s="29"/>
+      <c r="E157" s="29"/>
     </row>
     <row r="483" spans="1:6" customHeight="1" ht="28">
       <c r="B483" s="36" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C483" s="37" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D483" s="37" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E483" s="37" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="484" spans="1:6">
       <c r="B484" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C484" s="38">
-        <v>12</v>
-      </c>
-      <c r="D484" s="38">
-        <v>12</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C484" s="38"/>
+      <c r="D484" s="38"/>
       <c r="E484" s="38"/>
     </row>
     <row r="485" spans="1:6">
       <c r="B485" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C485" s="38">
-        <v>17</v>
-      </c>
-      <c r="D485" s="38">
-        <v>189</v>
-      </c>
-      <c r="E485" s="38">
-        <v>189</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C485" s="38"/>
+      <c r="D485" s="38"/>
+      <c r="E485" s="38"/>
     </row>
     <row r="493" spans="1:6">
       <c r="C493" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="D493" s="52">
-        <v>12</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D493" s="52"/>
       <c r="E493" s="50"/>
       <c r="F493" s="50"/>
     </row>
     <row r="494" spans="1:6">
       <c r="C494" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="D494" s="52">
-        <v>45</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D494" s="52"/>
       <c r="E494" s="50"/>
       <c r="F494" s="50"/>
     </row>
     <row r="495" spans="1:6">
       <c r="C495" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="D495" s="52">
-        <v>87</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D495" s="52"/>
       <c r="E495" s="50"/>
       <c r="F495" s="50"/>
     </row>
     <row r="496" spans="1:6">
       <c r="C496" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="D496" s="52">
-        <v>46</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D496" s="52"/>
       <c r="E496" s="50"/>
       <c r="F496" s="50"/>
     </row>
@@ -1831,41 +1710,33 @@
     </row>
     <row r="504" spans="1:6">
       <c r="C504" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="D504" s="52">
-        <v>12</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D504" s="52"/>
       <c r="E504" s="50"/>
       <c r="F504" s="50"/>
     </row>
     <row r="505" spans="1:6">
       <c r="C505" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="D505" s="52">
-        <v>23</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D505" s="52"/>
       <c r="E505" s="50"/>
       <c r="F505" s="50"/>
     </row>
     <row r="506" spans="1:6">
       <c r="C506" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="D506" s="52">
-        <v>67</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D506" s="52"/>
       <c r="E506" s="50"/>
       <c r="F506" s="50"/>
     </row>
     <row r="507" spans="1:6">
       <c r="C507" s="51" t="s">
-        <v>61</v>
-      </c>
-      <c r="D507" s="52">
-        <v>35</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D507" s="52"/>
       <c r="E507" s="50"/>
       <c r="F507" s="50"/>
     </row>
@@ -1913,50 +1784,38 @@
     </row>
     <row r="515" spans="1:6">
       <c r="C515" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D515" s="29" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E515" s="29" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F515" s="50"/>
     </row>
     <row r="516" spans="1:6">
       <c r="C516" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="D516" s="53">
-        <v>176</v>
-      </c>
-      <c r="E516" s="54">
         <v>56</v>
       </c>
+      <c r="D516" s="53"/>
+      <c r="E516" s="54"/>
       <c r="F516" s="50"/>
     </row>
     <row r="517" spans="1:6">
       <c r="C517" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D517" s="53">
-        <v>178</v>
-      </c>
-      <c r="E517" s="54">
-        <v>87</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D517" s="53"/>
+      <c r="E517" s="54"/>
       <c r="F517" s="50"/>
     </row>
     <row r="518" spans="1:6">
       <c r="C518" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D518" s="53">
-        <v>12</v>
-      </c>
-      <c r="E518" s="54">
-        <v>17</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D518" s="53"/>
+      <c r="E518" s="54"/>
       <c r="F518" s="50"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in slot no
</commit_message>
<xml_diff>
--- a/phpdocx/template/graph_excel.xlsx
+++ b/phpdocx/template/graph_excel.xlsx
@@ -977,46 +977,86 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="C4" s="3">
+        <v>2015</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2014</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2013</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2012</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="C5" s="5">
+        <v>17.4</v>
+      </c>
+      <c r="D5" s="5">
+        <v>17.42</v>
+      </c>
+      <c r="E5" s="5">
+        <v>17.44</v>
+      </c>
+      <c r="F5" s="5">
+        <v>7.93</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="C7" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2.08</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1.65</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1.89</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="C8" s="5">
+        <v>80.1</v>
+      </c>
+      <c r="D8" s="5">
+        <v>80.5</v>
+      </c>
+      <c r="E8" s="5">
+        <v>80.91</v>
+      </c>
+      <c r="F8" s="5">
+        <v>90.18</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="6" t="s">

</xml_diff>

<commit_message>
fixed excel burning issues
</commit_message>
<xml_diff>
--- a/phpdocx/template/graph_excel.xlsx
+++ b/phpdocx/template/graph_excel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
   <si>
     <t>Shareholding Pattern</t>
   </si>
@@ -74,6 +74,9 @@
     <t>Non-Executive</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>Non-Promoter</t>
   </si>
   <si>
@@ -104,7 +107,13 @@
     <t>Non Audit</t>
   </si>
   <si>
-    <t>FY -1/0</t>
+    <t>FY 12/13</t>
+  </si>
+  <si>
+    <t>FY 13/14</t>
+  </si>
+  <si>
+    <t>FY 14/15</t>
   </si>
   <si>
     <t>Audit Fee</t>
@@ -125,7 +134,13 @@
     <t>Net Profit</t>
   </si>
   <si>
-    <t>FY -1/</t>
+    <t>FY 11/12</t>
+  </si>
+  <si>
+    <t>FY 10/11</t>
+  </si>
+  <si>
+    <t>FY 9/10</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -146,6 +161,12 @@
     <t>Total Commission</t>
   </si>
   <si>
+    <t>S&amp;P CNX Nifty</t>
+  </si>
+  <si>
+    <t>CNX Finance</t>
+  </si>
+  <si>
     <t>Today</t>
   </si>
   <si>
@@ -167,7 +188,16 @@
     <t>Proposed increase</t>
   </si>
   <si>
-    <t>'</t>
+    <t>Dec'15</t>
+  </si>
+  <si>
+    <t>Dec'14</t>
+  </si>
+  <si>
+    <t>Dec'13</t>
+  </si>
+  <si>
+    <t>Dec'12</t>
   </si>
   <si>
     <t>CSR</t>
@@ -995,16 +1025,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>17.4</v>
+        <v>53.05</v>
       </c>
       <c r="D5" s="5">
-        <v>17.42</v>
+        <v>53.05</v>
       </c>
       <c r="E5" s="5">
-        <v>17.44</v>
+        <v>53.05</v>
       </c>
       <c r="F5" s="5">
-        <v>7.93</v>
+        <v>53.05</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1012,16 +1042,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="5">
-        <v>0</v>
+        <v>1.03</v>
       </c>
       <c r="D6" s="5">
-        <v>0</v>
+        <v>0.79</v>
       </c>
       <c r="E6" s="5">
-        <v>0</v>
+        <v>1.35</v>
       </c>
       <c r="F6" s="5">
-        <v>0</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1029,16 +1059,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="5">
-        <v>2.5</v>
+        <v>19.26</v>
       </c>
       <c r="D7" s="5">
-        <v>2.08</v>
+        <v>20.9</v>
       </c>
       <c r="E7" s="5">
-        <v>1.65</v>
+        <v>17.73</v>
       </c>
       <c r="F7" s="5">
-        <v>1.89</v>
+        <v>13.39</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1046,16 +1076,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="5">
-        <v>80.1</v>
+        <v>26.66</v>
       </c>
       <c r="D8" s="5">
-        <v>80.5</v>
+        <v>25.26</v>
       </c>
       <c r="E8" s="5">
-        <v>80.91</v>
+        <v>27.87</v>
       </c>
       <c r="F8" s="5">
-        <v>90.18</v>
+        <v>31.99</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1068,19 +1098,25 @@
       <c r="B16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="8"/>
+      <c r="C16" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="B17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="8">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" s="46"/>
@@ -1096,10 +1132,10 @@
         <v>10</v>
       </c>
       <c r="C28" s="49">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="D28" s="49">
-        <v>0</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1107,10 +1143,10 @@
         <v>11</v>
       </c>
       <c r="C29" s="49">
-        <v>0</v>
+        <v>0.55</v>
       </c>
       <c r="D29" s="49">
-        <v>0</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1138,29 +1174,59 @@
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="B38" s="12"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="13"/>
+      <c r="B38" s="12">
+        <v>2011</v>
+      </c>
+      <c r="C38" s="19">
+        <v>2.5725</v>
+      </c>
+      <c r="D38" s="13">
+        <v>234.16</v>
+      </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="B39" s="12"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="13"/>
+      <c r="B39" s="12">
+        <v>2012</v>
+      </c>
+      <c r="C39" s="19">
+        <v>3.1618</v>
+      </c>
+      <c r="D39" s="13">
+        <v>277.4</v>
+      </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="B40" s="12"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="13"/>
+      <c r="B40" s="12">
+        <v>2013</v>
+      </c>
+      <c r="C40" s="19">
+        <v>3.8915</v>
+      </c>
+      <c r="D40" s="13">
+        <v>309.99</v>
+      </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="B41" s="12"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="13"/>
+      <c r="B41" s="12">
+        <v>2014</v>
+      </c>
+      <c r="C41" s="19">
+        <v>4.4698</v>
+      </c>
+      <c r="D41" s="13">
+        <v>318.74</v>
+      </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="B42" s="14"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="15"/>
+      <c r="B42" s="14">
+        <v>2015</v>
+      </c>
+      <c r="C42" s="20">
+        <v>4.9126</v>
+      </c>
+      <c r="D42" s="15">
+        <v>461.98</v>
+      </c>
     </row>
     <row r="48" spans="1:6">
       <c r="B48" t="s">
@@ -1180,357 +1246,541 @@
       <c r="B50" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="18"/>
+      <c r="C50" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="18">
+        <v>0.26</v>
+      </c>
     </row>
     <row r="51" spans="1:6">
       <c r="B51" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="18"/>
+        <v>20</v>
+      </c>
+      <c r="C51" s="17">
+        <v>4.91</v>
+      </c>
+      <c r="D51" s="18">
+        <v>0.36</v>
+      </c>
     </row>
     <row r="59" spans="1:6">
       <c r="B59" s="39"/>
       <c r="C59" s="40" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D59" s="40" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E59" s="40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="B60" s="40"/>
-      <c r="C60" s="41"/>
-      <c r="D60" s="42"/>
-      <c r="E60" s="43"/>
+      <c r="B60" s="40">
+        <v>2013</v>
+      </c>
+      <c r="C60" s="41">
+        <v>2.1</v>
+      </c>
+      <c r="D60" s="42">
+        <v>8.17</v>
+      </c>
+      <c r="E60" s="43">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="B61" s="40"/>
-      <c r="C61" s="41"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="43"/>
+      <c r="B61" s="40">
+        <v>2014</v>
+      </c>
+      <c r="C61" s="41">
+        <v>2.1</v>
+      </c>
+      <c r="D61" s="42">
+        <v>8.35</v>
+      </c>
+      <c r="E61" s="43">
+        <v>0.29</v>
+      </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="B62" s="40"/>
-      <c r="C62" s="41"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="43"/>
+      <c r="B62" s="40">
+        <v>2015</v>
+      </c>
+      <c r="C62" s="41">
+        <v>2.3</v>
+      </c>
+      <c r="D62" s="42">
+        <v>9.27</v>
+      </c>
+      <c r="E62" s="43">
+        <v>0.29</v>
+      </c>
     </row>
     <row r="71" spans="1:6">
       <c r="B71" s="40" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C71" s="40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D71" s="40" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="B72" s="41"/>
-      <c r="C72" s="41"/>
-      <c r="D72" s="43"/>
+      <c r="B72" s="41">
+        <v>2.3</v>
+      </c>
+      <c r="C72" s="41">
+        <v>9.27</v>
+      </c>
+      <c r="D72" s="43">
+        <v>0.29</v>
+      </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="B73" s="41"/>
-      <c r="C73" s="41"/>
-      <c r="D73" s="43"/>
+      <c r="B73" s="41">
+        <v>1</v>
+      </c>
+      <c r="C73" s="41">
+        <v>3.9</v>
+      </c>
+      <c r="D73" s="43">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="B74" s="41"/>
-      <c r="C74" s="41"/>
-      <c r="D74" s="43"/>
+      <c r="B74" s="41">
+        <v>3.2</v>
+      </c>
+      <c r="C74" s="41">
+        <v>21.12</v>
+      </c>
+      <c r="D74" s="43">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="82" spans="1:6">
       <c r="B82" s="21"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="22"/>
+      <c r="C82" s="22">
+        <v>2015</v>
+      </c>
+      <c r="D82" s="22">
+        <v>2014</v>
+      </c>
     </row>
     <row r="83" spans="1:6">
       <c r="B83" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C83" s="24"/>
-      <c r="D83" s="24"/>
+        <v>27</v>
+      </c>
+      <c r="C83" s="24">
+        <v>1.22</v>
+      </c>
+      <c r="D83" s="24">
+        <v>1.22</v>
+      </c>
     </row>
     <row r="84" spans="1:6">
       <c r="B84" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
+        <v>28</v>
+      </c>
+      <c r="C84" s="24">
+        <v>0.41</v>
+      </c>
+      <c r="D84" s="24">
+        <v>0.38</v>
+      </c>
     </row>
     <row r="85" spans="1:6">
       <c r="B85" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
+        <v>29</v>
+      </c>
+      <c r="C85" s="24">
+        <v>0.29</v>
+      </c>
+      <c r="D85" s="24">
+        <v>0.33</v>
+      </c>
     </row>
     <row r="95" spans="1:6" customHeight="1" ht="15"/>
     <row r="96" spans="1:6">
       <c r="B96" s="25"/>
       <c r="C96" s="26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E96" s="27" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="B97" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C97" s="29"/>
-      <c r="D97" s="29"/>
-      <c r="E97" s="30"/>
+        <v>33</v>
+      </c>
+      <c r="C97" s="29">
+        <v>1.02</v>
+      </c>
+      <c r="D97" s="29">
+        <v>1.22</v>
+      </c>
+      <c r="E97" s="30">
+        <v>1.22</v>
+      </c>
     </row>
     <row r="98" spans="1:6">
       <c r="B98" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C98" s="29"/>
-      <c r="D98" s="29"/>
-      <c r="E98" s="30"/>
+        <v>34</v>
+      </c>
+      <c r="C98" s="29">
+        <v>0.362</v>
+      </c>
+      <c r="D98" s="29">
+        <v>0.38</v>
+      </c>
+      <c r="E98" s="30">
+        <v>0.41</v>
+      </c>
     </row>
     <row r="99" spans="1:6" customHeight="1" ht="15">
       <c r="B99" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C99" s="32"/>
-      <c r="D99" s="32"/>
-      <c r="E99" s="33"/>
+        <v>35</v>
+      </c>
+      <c r="C99" s="32">
+        <v>0.28</v>
+      </c>
+      <c r="D99" s="32">
+        <v>0.33</v>
+      </c>
+      <c r="E99" s="33">
+        <v>0.29</v>
+      </c>
     </row>
     <row r="108" spans="1:6" customHeight="1" ht="15"/>
     <row r="109" spans="1:6">
       <c r="B109" s="25"/>
       <c r="C109" s="26" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D109" s="26" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E109" s="27" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="B110" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C110" s="29"/>
-      <c r="D110" s="29"/>
-      <c r="E110" s="30"/>
+        <v>32</v>
+      </c>
+      <c r="C110" s="29">
+        <v>4.9126</v>
+      </c>
+      <c r="D110" s="29">
+        <v>461.98</v>
+      </c>
+      <c r="E110" s="30">
+        <v>823.07</v>
+      </c>
     </row>
     <row r="111" spans="1:6">
       <c r="B111" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C111" s="29"/>
-      <c r="D111" s="29"/>
-      <c r="E111" s="30"/>
+        <v>31</v>
+      </c>
+      <c r="C111" s="29">
+        <v>4.4698</v>
+      </c>
+      <c r="D111" s="29">
+        <v>318.74</v>
+      </c>
+      <c r="E111" s="30">
+        <v>741.14</v>
+      </c>
     </row>
     <row r="112" spans="1:6">
       <c r="B112" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C112" s="29"/>
-      <c r="D112" s="29"/>
-      <c r="E112" s="30"/>
+        <v>30</v>
+      </c>
+      <c r="C112" s="29">
+        <v>3.8915</v>
+      </c>
+      <c r="D112" s="29">
+        <v>309.99</v>
+      </c>
+      <c r="E112" s="30">
+        <v>725.18</v>
+      </c>
     </row>
     <row r="113" spans="1:6">
       <c r="B113" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C113" s="29"/>
-      <c r="D113" s="29"/>
-      <c r="E113" s="30"/>
+        <v>39</v>
+      </c>
+      <c r="C113" s="29">
+        <v>3.1618</v>
+      </c>
+      <c r="D113" s="29">
+        <v>277.4</v>
+      </c>
+      <c r="E113" s="30">
+        <v>600.16</v>
+      </c>
     </row>
     <row r="114" spans="1:6" customHeight="1" ht="15">
       <c r="B114" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C114" s="32"/>
-      <c r="D114" s="32"/>
-      <c r="E114" s="30"/>
+        <v>40</v>
+      </c>
+      <c r="C114" s="32">
+        <v>2.5725</v>
+      </c>
+      <c r="D114" s="32">
+        <v>234.16</v>
+      </c>
+      <c r="E114" s="30">
+        <v>432.61</v>
+      </c>
     </row>
     <row r="115" spans="1:6" customHeight="1" ht="15">
       <c r="B115" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C115" s="32"/>
-      <c r="D115" s="32"/>
-      <c r="E115" s="33"/>
+        <v>41</v>
+      </c>
+      <c r="C115" s="32">
+        <v>0</v>
+      </c>
+      <c r="D115" s="32">
+        <v>0</v>
+      </c>
+      <c r="E115" s="33">
+        <v>0</v>
+      </c>
     </row>
     <row r="122" spans="1:6">
       <c r="C122" s="29" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D122" s="29" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="C123" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D123" s="34"/>
+        <v>44</v>
+      </c>
+      <c r="D123" s="34">
+        <v>24.96</v>
+      </c>
     </row>
     <row r="124" spans="1:6">
       <c r="C124" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D124" s="34"/>
+        <v>45</v>
+      </c>
+      <c r="D124" s="34">
+        <v>34.49</v>
+      </c>
     </row>
     <row r="125" spans="1:6">
       <c r="C125" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D125" s="34"/>
+        <v>46</v>
+      </c>
+      <c r="D125" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="29" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="C134" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D134" s="34"/>
+        <v>40</v>
+      </c>
+      <c r="D134" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="135" spans="1:6">
       <c r="C135" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D135" s="34"/>
+        <v>39</v>
+      </c>
+      <c r="D135" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="136" spans="1:6">
       <c r="C136" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D136" s="34"/>
+        <v>30</v>
+      </c>
+      <c r="D136" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="137" spans="1:6">
       <c r="C137" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D137" s="34"/>
+        <v>31</v>
+      </c>
+      <c r="D137" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="138" spans="1:6">
       <c r="C138" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D138" s="34"/>
+        <v>32</v>
+      </c>
+      <c r="D138" s="34">
+        <v>30.68</v>
+      </c>
     </row>
     <row r="153" spans="1:6">
       <c r="B153" s="29"/>
-      <c r="C153" s="29"/>
-      <c r="D153" s="29"/>
-      <c r="E153" s="29"/>
+      <c r="C153" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D153" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E153" s="29" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="154" spans="1:6">
       <c r="B154" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C154" s="29"/>
-      <c r="D154" s="29"/>
-      <c r="E154" s="29"/>
+        <v>50</v>
+      </c>
+      <c r="C154" s="29">
+        <v>90</v>
+      </c>
+      <c r="D154" s="29">
+        <v>234</v>
+      </c>
+      <c r="E154" s="29">
+        <v>354</v>
+      </c>
     </row>
     <row r="155" spans="1:6">
       <c r="B155" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C155" s="29"/>
-      <c r="D155" s="29"/>
-      <c r="E155" s="29"/>
+        <v>51</v>
+      </c>
+      <c r="C155" s="29">
+        <v>100</v>
+      </c>
+      <c r="D155" s="29">
+        <v>213</v>
+      </c>
+      <c r="E155" s="29">
+        <v>298</v>
+      </c>
     </row>
     <row r="156" spans="1:6">
       <c r="B156" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="C156" s="29"/>
-      <c r="D156" s="29"/>
-      <c r="E156" s="29"/>
+        <v>52</v>
+      </c>
+      <c r="C156" s="29">
+        <v>130</v>
+      </c>
+      <c r="D156" s="29">
+        <v>235</v>
+      </c>
+      <c r="E156" s="29">
+        <v>675</v>
+      </c>
     </row>
     <row r="157" spans="1:6">
       <c r="B157" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="C157" s="29"/>
-      <c r="D157" s="29"/>
-      <c r="E157" s="29"/>
+        <v>53</v>
+      </c>
+      <c r="C157" s="29">
+        <v>140</v>
+      </c>
+      <c r="D157" s="29">
+        <v>987</v>
+      </c>
+      <c r="E157" s="29">
+        <v>283</v>
+      </c>
     </row>
     <row r="483" spans="1:6" customHeight="1" ht="28">
       <c r="B483" s="36" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C483" s="37" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D483" s="37" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="E483" s="37" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="484" spans="1:6">
       <c r="B484" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C484" s="38"/>
-      <c r="D484" s="38"/>
+        <v>57</v>
+      </c>
+      <c r="C484" s="38">
+        <v>123</v>
+      </c>
+      <c r="D484" s="38">
+        <v>216</v>
+      </c>
       <c r="E484" s="38"/>
     </row>
     <row r="485" spans="1:6">
       <c r="B485" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C485" s="38"/>
-      <c r="D485" s="38"/>
-      <c r="E485" s="38"/>
+        <v>58</v>
+      </c>
+      <c r="C485" s="38">
+        <v>187</v>
+      </c>
+      <c r="D485" s="38">
+        <v>987</v>
+      </c>
+      <c r="E485" s="38">
+        <v>1009</v>
+      </c>
     </row>
     <row r="493" spans="1:6">
       <c r="C493" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D493" s="52"/>
+        <v>57</v>
+      </c>
+      <c r="D493" s="52">
+        <v>23</v>
+      </c>
       <c r="E493" s="50"/>
       <c r="F493" s="50"/>
     </row>
     <row r="494" spans="1:6">
       <c r="C494" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D494" s="52"/>
+        <v>58</v>
+      </c>
+      <c r="D494" s="52">
+        <v>24</v>
+      </c>
       <c r="E494" s="50"/>
       <c r="F494" s="50"/>
     </row>
     <row r="495" spans="1:6">
       <c r="C495" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D495" s="52"/>
+        <v>59</v>
+      </c>
+      <c r="D495" s="52">
+        <v>26.5</v>
+      </c>
       <c r="E495" s="50"/>
       <c r="F495" s="50"/>
     </row>
     <row r="496" spans="1:6">
       <c r="C496" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D496" s="52"/>
+        <v>60</v>
+      </c>
+      <c r="D496" s="52">
+        <v>21.87</v>
+      </c>
       <c r="E496" s="50"/>
       <c r="F496" s="50"/>
     </row>
@@ -1578,33 +1828,41 @@
     </row>
     <row r="504" spans="1:6">
       <c r="C504" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D504" s="52"/>
+        <v>57</v>
+      </c>
+      <c r="D504" s="52">
+        <v>12.34</v>
+      </c>
       <c r="E504" s="50"/>
       <c r="F504" s="50"/>
     </row>
     <row r="505" spans="1:6">
       <c r="C505" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D505" s="52"/>
+        <v>57</v>
+      </c>
+      <c r="D505" s="52">
+        <v>21.21</v>
+      </c>
       <c r="E505" s="50"/>
       <c r="F505" s="50"/>
     </row>
     <row r="506" spans="1:6">
       <c r="C506" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D506" s="52"/>
+        <v>57</v>
+      </c>
+      <c r="D506" s="52">
+        <v>12.34</v>
+      </c>
       <c r="E506" s="50"/>
       <c r="F506" s="50"/>
     </row>
     <row r="507" spans="1:6">
       <c r="C507" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D507" s="52"/>
+        <v>57</v>
+      </c>
+      <c r="D507" s="52">
+        <v>64.32</v>
+      </c>
       <c r="E507" s="50"/>
       <c r="F507" s="50"/>
     </row>
@@ -1652,100 +1910,148 @@
     </row>
     <row r="515" spans="1:6">
       <c r="C515" s="29" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D515" s="29" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E515" s="29" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="F515" s="50"/>
     </row>
     <row r="516" spans="1:6">
       <c r="C516" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D516" s="53"/>
-      <c r="E516" s="54"/>
+        <v>30</v>
+      </c>
+      <c r="D516" s="53">
+        <v>213</v>
+      </c>
+      <c r="E516" s="54">
+        <v>28</v>
+      </c>
       <c r="F516" s="50"/>
     </row>
     <row r="517" spans="1:6">
       <c r="C517" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D517" s="53"/>
-      <c r="E517" s="54"/>
+        <v>31</v>
+      </c>
+      <c r="D517" s="53">
+        <v>125</v>
+      </c>
+      <c r="E517" s="54">
+        <v>21</v>
+      </c>
       <c r="F517" s="50"/>
     </row>
     <row r="518" spans="1:6">
       <c r="C518" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D518" s="53"/>
-      <c r="E518" s="54"/>
+        <v>32</v>
+      </c>
+      <c r="D518" s="53">
+        <v>123</v>
+      </c>
+      <c r="E518" s="54">
+        <v>23</v>
+      </c>
       <c r="F518" s="50"/>
     </row>
     <row r="530" spans="1:6" customHeight="1" ht="15"/>
     <row r="531" spans="1:6">
       <c r="B531" s="25"/>
       <c r="C531" s="26" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D531" s="26" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E531" s="27" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="532" spans="1:6">
       <c r="B532" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C532" s="29"/>
-      <c r="D532" s="29"/>
-      <c r="E532" s="30"/>
+        <v>32</v>
+      </c>
+      <c r="C532" s="29">
+        <v>4.9126</v>
+      </c>
+      <c r="D532" s="29">
+        <v>461.98</v>
+      </c>
+      <c r="E532" s="30">
+        <v>823.07</v>
+      </c>
     </row>
     <row r="533" spans="1:6">
       <c r="B533" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C533" s="29"/>
-      <c r="D533" s="29"/>
-      <c r="E533" s="30"/>
+        <v>31</v>
+      </c>
+      <c r="C533" s="29">
+        <v>4.4698</v>
+      </c>
+      <c r="D533" s="29">
+        <v>318.74</v>
+      </c>
+      <c r="E533" s="30">
+        <v>741.14</v>
+      </c>
     </row>
     <row r="534" spans="1:6">
       <c r="B534" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C534" s="29"/>
-      <c r="D534" s="29"/>
-      <c r="E534" s="30"/>
+        <v>30</v>
+      </c>
+      <c r="C534" s="29">
+        <v>3.8915</v>
+      </c>
+      <c r="D534" s="29">
+        <v>309.99</v>
+      </c>
+      <c r="E534" s="30">
+        <v>725.18</v>
+      </c>
     </row>
     <row r="535" spans="1:6">
       <c r="B535" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C535" s="29"/>
-      <c r="D535" s="29"/>
-      <c r="E535" s="30"/>
+        <v>39</v>
+      </c>
+      <c r="C535" s="29">
+        <v>3.1618</v>
+      </c>
+      <c r="D535" s="29">
+        <v>277.4</v>
+      </c>
+      <c r="E535" s="30">
+        <v>600.16</v>
+      </c>
     </row>
     <row r="536" spans="1:6" customHeight="1" ht="15">
       <c r="B536" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C536" s="32"/>
-      <c r="D536" s="32"/>
-      <c r="E536" s="30"/>
+        <v>40</v>
+      </c>
+      <c r="C536" s="32">
+        <v>2.5725</v>
+      </c>
+      <c r="D536" s="32">
+        <v>234.16</v>
+      </c>
+      <c r="E536" s="30">
+        <v>432.61</v>
+      </c>
     </row>
     <row r="537" spans="1:6" customHeight="1" ht="15">
       <c r="B537" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C537" s="32"/>
-      <c r="D537" s="32"/>
-      <c r="E537" s="33"/>
+        <v>41</v>
+      </c>
+      <c r="C537" s="32">
+        <v>0</v>
+      </c>
+      <c r="D537" s="32">
+        <v>0</v>
+      </c>
+      <c r="E537" s="33">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
appointment of auditors page fix company name
</commit_message>
<xml_diff>
--- a/phpdocx/template/graph_excel.xlsx
+++ b/phpdocx/template/graph_excel.xlsx
@@ -977,86 +977,46 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4" s="2"/>
-      <c r="C4" s="3">
-        <v>2015</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2014</v>
-      </c>
-      <c r="E4" s="3">
-        <v>2013</v>
-      </c>
-      <c r="F4" s="3">
-        <v>2012</v>
-      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
-        <v>17.4</v>
-      </c>
-      <c r="D5" s="5">
-        <v>17.42</v>
-      </c>
-      <c r="E5" s="5">
-        <v>17.44</v>
-      </c>
-      <c r="F5" s="5">
-        <v>7.93</v>
-      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0</v>
-      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="D7" s="5">
-        <v>2.08</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1.65</v>
-      </c>
-      <c r="F7" s="5">
-        <v>1.89</v>
-      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5">
-        <v>80.1</v>
-      </c>
-      <c r="D8" s="5">
-        <v>80.5</v>
-      </c>
-      <c r="E8" s="5">
-        <v>80.91</v>
-      </c>
-      <c r="F8" s="5">
-        <v>90.18</v>
-      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="6" t="s">

</xml_diff>

<commit_message>
change folder name docx file name in template folder and burning issues
</commit_message>
<xml_diff>
--- a/phpdocx/template/graph_excel.xlsx
+++ b/phpdocx/template/graph_excel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
   <si>
     <t>Shareholding Pattern</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Non-Executive</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
   <si>
     <t>Non-Promoter</t>
@@ -977,46 +980,86 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="C4" s="3">
+        <v>2015</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2014</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2013</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2012</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="C6" s="5">
+        <v>37.96</v>
+      </c>
+      <c r="D6" s="5">
+        <v>42.1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>40.52</v>
+      </c>
+      <c r="F6" s="5">
+        <v>39.02</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="C7" s="5">
+        <v>15.1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>-42.1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>17.51</v>
+      </c>
+      <c r="F7" s="5">
+        <v>16.57</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="C8" s="5">
+        <v>46.94</v>
+      </c>
+      <c r="D8" s="5">
+        <v>100</v>
+      </c>
+      <c r="E8" s="5">
+        <v>41.97</v>
+      </c>
+      <c r="F8" s="5">
+        <v>44.41</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="6" t="s">
@@ -1028,19 +1071,25 @@
       <c r="B16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="8"/>
+      <c r="C16" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="B17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" s="46"/>
@@ -1056,10 +1105,10 @@
         <v>10</v>
       </c>
       <c r="C28" s="49">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D28" s="49">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1067,10 +1116,10 @@
         <v>11</v>
       </c>
       <c r="C29" s="49">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D29" s="49">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1098,29 +1147,59 @@
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="B38" s="12"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="13"/>
+      <c r="B38" s="12">
+        <v>2011</v>
+      </c>
+      <c r="C38" s="19">
+        <v>0</v>
+      </c>
+      <c r="D38" s="13">
+        <v>125.66</v>
+      </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="B39" s="12"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="13"/>
+      <c r="B39" s="12">
+        <v>2012</v>
+      </c>
+      <c r="C39" s="19">
+        <v>0</v>
+      </c>
+      <c r="D39" s="13">
+        <v>115.26</v>
+      </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="B40" s="12"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="13"/>
+      <c r="B40" s="12">
+        <v>2013</v>
+      </c>
+      <c r="C40" s="19">
+        <v>0</v>
+      </c>
+      <c r="D40" s="13">
+        <v>119.33</v>
+      </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="B41" s="12"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="13"/>
+      <c r="B41" s="12">
+        <v>2014</v>
+      </c>
+      <c r="C41" s="19">
+        <v>0.83</v>
+      </c>
+      <c r="D41" s="13">
+        <v>138.61</v>
+      </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="B42" s="14"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="15"/>
+      <c r="B42" s="14">
+        <v>2015</v>
+      </c>
+      <c r="C42" s="20">
+        <v>6.08</v>
+      </c>
+      <c r="D42" s="15">
+        <v>186.28</v>
+      </c>
     </row>
     <row r="48" spans="1:6">
       <c r="B48" t="s">
@@ -1140,26 +1219,34 @@
       <c r="B50" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="18"/>
+      <c r="C50" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="51" spans="1:6">
       <c r="B51" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="18"/>
+        <v>20</v>
+      </c>
+      <c r="C51" s="17">
+        <v>5.32</v>
+      </c>
+      <c r="D51" s="18">
+        <v>0.87</v>
+      </c>
     </row>
     <row r="59" spans="1:6">
       <c r="B59" s="39"/>
       <c r="C59" s="40" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D59" s="40" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E59" s="40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1182,13 +1269,13 @@
     </row>
     <row r="71" spans="1:6">
       <c r="B71" s="40" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C71" s="40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D71" s="40" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1213,21 +1300,21 @@
     </row>
     <row r="83" spans="1:6">
       <c r="B83" s="23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C83" s="24"/>
       <c r="D83" s="24"/>
     </row>
     <row r="84" spans="1:6">
       <c r="B84" s="23" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C84" s="24"/>
       <c r="D84" s="24"/>
     </row>
     <row r="85" spans="1:6">
       <c r="B85" s="23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C85" s="24"/>
       <c r="D85" s="24"/>
@@ -1236,18 +1323,18 @@
     <row r="96" spans="1:6">
       <c r="B96" s="25"/>
       <c r="C96" s="26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E96" s="27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="B97" s="28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C97" s="29"/>
       <c r="D97" s="29"/>
@@ -1255,7 +1342,7 @@
     </row>
     <row r="98" spans="1:6">
       <c r="B98" s="28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C98" s="29"/>
       <c r="D98" s="29"/>
@@ -1263,7 +1350,7 @@
     </row>
     <row r="99" spans="1:6" customHeight="1" ht="15">
       <c r="B99" s="31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C99" s="32"/>
       <c r="D99" s="32"/>
@@ -1273,18 +1360,18 @@
     <row r="109" spans="1:6">
       <c r="B109" s="25"/>
       <c r="C109" s="26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D109" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E109" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="B110" s="28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C110" s="29"/>
       <c r="D110" s="29"/>
@@ -1292,7 +1379,7 @@
     </row>
     <row r="111" spans="1:6">
       <c r="B111" s="28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C111" s="29"/>
       <c r="D111" s="29"/>
@@ -1300,7 +1387,7 @@
     </row>
     <row r="112" spans="1:6">
       <c r="B112" s="28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C112" s="29"/>
       <c r="D112" s="29"/>
@@ -1308,7 +1395,7 @@
     </row>
     <row r="113" spans="1:6">
       <c r="B113" s="28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C113" s="29"/>
       <c r="D113" s="29"/>
@@ -1316,7 +1403,7 @@
     </row>
     <row r="114" spans="1:6" customHeight="1" ht="15">
       <c r="B114" s="28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C114" s="32"/>
       <c r="D114" s="32"/>
@@ -1324,7 +1411,7 @@
     </row>
     <row r="115" spans="1:6" customHeight="1" ht="15">
       <c r="B115" s="31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C115" s="32"/>
       <c r="D115" s="32"/>
@@ -1332,65 +1419,65 @@
     </row>
     <row r="122" spans="1:6">
       <c r="C122" s="29" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D122" s="29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="C123" s="29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D123" s="34"/>
     </row>
     <row r="124" spans="1:6">
       <c r="C124" s="29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D124" s="34"/>
     </row>
     <row r="125" spans="1:6">
       <c r="C125" s="29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D125" s="34"/>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="29" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="C134" s="29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D134" s="34"/>
     </row>
     <row r="135" spans="1:6">
       <c r="C135" s="29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D135" s="34"/>
     </row>
     <row r="136" spans="1:6">
       <c r="C136" s="29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D136" s="34"/>
     </row>
     <row r="137" spans="1:6">
       <c r="C137" s="29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D137" s="34"/>
     </row>
     <row r="138" spans="1:6">
       <c r="C138" s="29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D138" s="34"/>
     </row>
@@ -1402,7 +1489,7 @@
     </row>
     <row r="154" spans="1:6">
       <c r="B154" s="35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C154" s="29"/>
       <c r="D154" s="29"/>
@@ -1410,7 +1497,7 @@
     </row>
     <row r="155" spans="1:6">
       <c r="B155" s="35" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C155" s="29"/>
       <c r="D155" s="29"/>
@@ -1418,7 +1505,7 @@
     </row>
     <row r="156" spans="1:6">
       <c r="B156" s="35" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C156" s="29"/>
       <c r="D156" s="29"/>
@@ -1426,7 +1513,7 @@
     </row>
     <row r="157" spans="1:6">
       <c r="B157" s="35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C157" s="29"/>
       <c r="D157" s="29"/>
@@ -1434,21 +1521,21 @@
     </row>
     <row r="483" spans="1:6" customHeight="1" ht="28">
       <c r="B483" s="36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C483" s="37" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D483" s="37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E483" s="37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="484" spans="1:6">
       <c r="B484" s="29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C484" s="38"/>
       <c r="D484" s="38"/>
@@ -1456,7 +1543,7 @@
     </row>
     <row r="485" spans="1:6">
       <c r="B485" s="29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C485" s="38"/>
       <c r="D485" s="38"/>
@@ -1464,7 +1551,7 @@
     </row>
     <row r="493" spans="1:6">
       <c r="C493" s="51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D493" s="52"/>
       <c r="E493" s="50"/>
@@ -1472,7 +1559,7 @@
     </row>
     <row r="494" spans="1:6">
       <c r="C494" s="51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D494" s="52"/>
       <c r="E494" s="50"/>
@@ -1480,7 +1567,7 @@
     </row>
     <row r="495" spans="1:6">
       <c r="C495" s="51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D495" s="52"/>
       <c r="E495" s="50"/>
@@ -1488,7 +1575,7 @@
     </row>
     <row r="496" spans="1:6">
       <c r="C496" s="51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D496" s="52"/>
       <c r="E496" s="50"/>
@@ -1538,7 +1625,7 @@
     </row>
     <row r="504" spans="1:6">
       <c r="C504" s="51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D504" s="52"/>
       <c r="E504" s="50"/>
@@ -1546,7 +1633,7 @@
     </row>
     <row r="505" spans="1:6">
       <c r="C505" s="51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D505" s="52"/>
       <c r="E505" s="50"/>
@@ -1554,7 +1641,7 @@
     </row>
     <row r="506" spans="1:6">
       <c r="C506" s="51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D506" s="52"/>
       <c r="E506" s="50"/>
@@ -1562,7 +1649,7 @@
     </row>
     <row r="507" spans="1:6">
       <c r="C507" s="51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D507" s="52"/>
       <c r="E507" s="50"/>
@@ -1612,19 +1699,19 @@
     </row>
     <row r="515" spans="1:6">
       <c r="C515" s="29" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D515" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E515" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F515" s="50"/>
     </row>
     <row r="516" spans="1:6">
       <c r="C516" s="29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D516" s="53"/>
       <c r="E516" s="54"/>
@@ -1632,7 +1719,7 @@
     </row>
     <row r="517" spans="1:6">
       <c r="C517" s="29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D517" s="53"/>
       <c r="E517" s="54"/>
@@ -1640,7 +1727,7 @@
     </row>
     <row r="518" spans="1:6">
       <c r="C518" s="29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D518" s="53"/>
       <c r="E518" s="54"/>
@@ -1650,18 +1737,18 @@
     <row r="531" spans="1:6">
       <c r="B531" s="25"/>
       <c r="C531" s="26" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D531" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E531" s="27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="532" spans="1:6">
       <c r="B532" s="28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C532" s="29"/>
       <c r="D532" s="29"/>
@@ -1669,7 +1756,7 @@
     </row>
     <row r="533" spans="1:6">
       <c r="B533" s="28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C533" s="29"/>
       <c r="D533" s="29"/>
@@ -1677,7 +1764,7 @@
     </row>
     <row r="534" spans="1:6">
       <c r="B534" s="28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C534" s="29"/>
       <c r="D534" s="29"/>
@@ -1685,7 +1772,7 @@
     </row>
     <row r="535" spans="1:6">
       <c r="B535" s="28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C535" s="29"/>
       <c r="D535" s="29"/>
@@ -1693,7 +1780,7 @@
     </row>
     <row r="536" spans="1:6" customHeight="1" ht="15">
       <c r="B536" s="28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C536" s="32"/>
       <c r="D536" s="32"/>
@@ -1701,7 +1788,7 @@
     </row>
     <row r="537" spans="1:6" customHeight="1" ht="15">
       <c r="B537" s="31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C537" s="32"/>
       <c r="D537" s="32"/>

</xml_diff>

<commit_message>
Fixed burning issues in director's remuneration
</commit_message>
<xml_diff>
--- a/phpdocx/template/graph_excel.xlsx
+++ b/phpdocx/template/graph_excel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
   <si>
     <t>Shareholding Pattern</t>
   </si>
@@ -74,12 +74,12 @@
     <t>Non-Executive</t>
   </si>
   <si>
+    <t>Non-Promoter</t>
+  </si>
+  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>Non-Promoter</t>
-  </si>
-  <si>
     <t>Dividend (LHS)</t>
   </si>
   <si>
@@ -107,76 +107,97 @@
     <t>Non Audit</t>
   </si>
   <si>
+    <t>FY 12/13</t>
+  </si>
+  <si>
+    <t>FY 13/14</t>
+  </si>
+  <si>
+    <t>FY 14/15</t>
+  </si>
+  <si>
+    <t>Audit Fee</t>
+  </si>
+  <si>
+    <t>Audit Related Fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non Audit Fee </t>
+  </si>
+  <si>
+    <t>ED Remuneration</t>
+  </si>
+  <si>
+    <t>Indexed TSR</t>
+  </si>
+  <si>
+    <t>Net Profit</t>
+  </si>
+  <si>
+    <t>FY 11/12</t>
+  </si>
+  <si>
+    <t>FY 10/11</t>
+  </si>
+  <si>
+    <t>FY 9/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Commission</t>
+  </si>
+  <si>
+    <t>Promoter NED</t>
+  </si>
+  <si>
+    <t>Independent Directors</t>
+  </si>
+  <si>
+    <t>Other NEDs</t>
+  </si>
+  <si>
+    <t>Total Commission</t>
+  </si>
+  <si>
+    <t>FY -1/</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>1Y</t>
+  </si>
+  <si>
+    <t>3Y</t>
+  </si>
+  <si>
+    <t>5Y</t>
+  </si>
+  <si>
+    <t>Existing Borrowing</t>
+  </si>
+  <si>
+    <t>Unavailed borrowing limit</t>
+  </si>
+  <si>
+    <t>Proposed increase</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>CSR</t>
+  </si>
+  <si>
+    <t>CSR as % of Net Profit</t>
+  </si>
+  <si>
     <t>FY -1/0</t>
   </si>
   <si>
-    <t>Audit Fee</t>
-  </si>
-  <si>
-    <t>Audit Related Fee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non Audit Fee </t>
-  </si>
-  <si>
-    <t>ED Remuneration</t>
-  </si>
-  <si>
-    <t>Indexed TSR</t>
-  </si>
-  <si>
-    <t>Net Profit</t>
-  </si>
-  <si>
-    <t>FY -1/</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Commission</t>
-  </si>
-  <si>
-    <t>Promoter NED</t>
-  </si>
-  <si>
-    <t>Independent Directors</t>
-  </si>
-  <si>
-    <t>Other NEDs</t>
-  </si>
-  <si>
-    <t>Total Commission</t>
-  </si>
-  <si>
-    <t>Today</t>
-  </si>
-  <si>
-    <t>1Y</t>
-  </si>
-  <si>
-    <t>3Y</t>
-  </si>
-  <si>
-    <t>5Y</t>
-  </si>
-  <si>
-    <t>Existing Borrowing</t>
-  </si>
-  <si>
-    <t>Unavailed borrowing limit</t>
-  </si>
-  <si>
-    <t>Proposed increase</t>
-  </si>
-  <si>
-    <t>'</t>
-  </si>
-  <si>
-    <t>CSR</t>
-  </si>
-  <si>
-    <t>CSR as % of Net Profit</t>
+    <t>FY -1/00</t>
   </si>
 </sst>
 </file>
@@ -998,16 +1019,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>0</v>
+        <v>52.35</v>
       </c>
       <c r="D5" s="5">
-        <v>0</v>
+        <v>52.35</v>
       </c>
       <c r="E5" s="5">
-        <v>0</v>
+        <v>52.29</v>
       </c>
       <c r="F5" s="5">
-        <v>0</v>
+        <v>52.07</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1015,16 +1036,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="5">
-        <v>37.96</v>
+        <v>8.31</v>
       </c>
       <c r="D6" s="5">
-        <v>42.1</v>
+        <v>8.14</v>
       </c>
       <c r="E6" s="5">
-        <v>40.52</v>
+        <v>9.5</v>
       </c>
       <c r="F6" s="5">
-        <v>39.02</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1032,16 +1053,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="5">
-        <v>15.1</v>
+        <v>9.94</v>
       </c>
       <c r="D7" s="5">
-        <v>-42.1</v>
+        <v>11.64</v>
       </c>
       <c r="E7" s="5">
-        <v>17.51</v>
+        <v>15.61</v>
       </c>
       <c r="F7" s="5">
-        <v>16.57</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1049,16 +1070,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="5">
-        <v>46.94</v>
+        <v>29.4</v>
       </c>
       <c r="D8" s="5">
-        <v>100</v>
+        <v>27.87</v>
       </c>
       <c r="E8" s="5">
-        <v>41.97</v>
+        <v>22.6</v>
       </c>
       <c r="F8" s="5">
-        <v>44.41</v>
+        <v>21.93</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1080,7 +1101,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1088,7 +1109,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="8">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1105,10 +1126,10 @@
         <v>10</v>
       </c>
       <c r="C28" s="49">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="D28" s="49">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1116,10 +1137,10 @@
         <v>11</v>
       </c>
       <c r="C29" s="49">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="D29" s="49">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1151,10 +1172,10 @@
         <v>2011</v>
       </c>
       <c r="C38" s="19">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="D38" s="13">
-        <v>125.66</v>
+        <v>68.18</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1162,10 +1183,10 @@
         <v>2012</v>
       </c>
       <c r="C39" s="19">
-        <v>0</v>
+        <v>3.88</v>
       </c>
       <c r="D39" s="13">
-        <v>115.26</v>
+        <v>109.13</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1173,10 +1194,10 @@
         <v>2013</v>
       </c>
       <c r="C40" s="19">
-        <v>0</v>
+        <v>5.12</v>
       </c>
       <c r="D40" s="13">
-        <v>119.33</v>
+        <v>85.04</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1184,10 +1205,10 @@
         <v>2014</v>
       </c>
       <c r="C41" s="19">
-        <v>0.83</v>
+        <v>5.38</v>
       </c>
       <c r="D41" s="13">
-        <v>138.61</v>
+        <v>57.51</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1195,10 +1216,10 @@
         <v>2015</v>
       </c>
       <c r="C42" s="20">
-        <v>6.08</v>
+        <v>5.62</v>
       </c>
       <c r="D42" s="15">
-        <v>186.28</v>
+        <v>65.75</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1219,22 +1240,22 @@
       <c r="B50" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>19</v>
+      <c r="C50" s="17">
+        <v>5.62</v>
+      </c>
+      <c r="D50" s="18">
+        <v>0.03</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="B51" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="17">
-        <v>5.32</v>
-      </c>
       <c r="D51" s="18">
-        <v>0.87</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1250,22 +1271,46 @@
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="B60" s="40"/>
-      <c r="C60" s="41"/>
-      <c r="D60" s="42"/>
-      <c r="E60" s="43"/>
+      <c r="B60" s="40">
+        <v>2013</v>
+      </c>
+      <c r="C60" s="41">
+        <v>1</v>
+      </c>
+      <c r="D60" s="42">
+        <v>3.67</v>
+      </c>
+      <c r="E60" s="43">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="B61" s="40"/>
-      <c r="C61" s="41"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="43"/>
+      <c r="B61" s="40">
+        <v>2014</v>
+      </c>
+      <c r="C61" s="41">
+        <v>0.8</v>
+      </c>
+      <c r="D61" s="42">
+        <v>1.18</v>
+      </c>
+      <c r="E61" s="43">
+        <v>0.79</v>
+      </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="B62" s="40"/>
-      <c r="C62" s="41"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="43"/>
+      <c r="B62" s="40">
+        <v>2015</v>
+      </c>
+      <c r="C62" s="41">
+        <v>0.8</v>
+      </c>
+      <c r="D62" s="42">
+        <v>1.19</v>
+      </c>
+      <c r="E62" s="43">
+        <v>0.78</v>
+      </c>
     </row>
     <row r="71" spans="1:6">
       <c r="B71" s="40" t="s">
@@ -1279,45 +1324,79 @@
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="B72" s="41"/>
-      <c r="C72" s="41"/>
-      <c r="D72" s="43"/>
+      <c r="B72" s="41">
+        <v>0.8</v>
+      </c>
+      <c r="C72" s="41">
+        <v>1.19</v>
+      </c>
+      <c r="D72" s="43">
+        <v>0.78</v>
+      </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="B73" s="41"/>
-      <c r="C73" s="41"/>
-      <c r="D73" s="43"/>
+      <c r="B73" s="41">
+        <v>10</v>
+      </c>
+      <c r="C73" s="41">
+        <v>56.42</v>
+      </c>
+      <c r="D73" s="43">
+        <v>0.21</v>
+      </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="B74" s="41"/>
-      <c r="C74" s="41"/>
-      <c r="D74" s="43"/>
+      <c r="B74" s="41">
+        <v>3</v>
+      </c>
+      <c r="C74" s="41">
+        <v>16.29</v>
+      </c>
+      <c r="D74" s="43">
+        <v>0.21</v>
+      </c>
     </row>
     <row r="82" spans="1:6">
       <c r="B82" s="21"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="22"/>
+      <c r="C82" s="22">
+        <v>2015</v>
+      </c>
+      <c r="D82" s="22">
+        <v>2014</v>
+      </c>
     </row>
     <row r="83" spans="1:6">
       <c r="B83" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C83" s="24"/>
-      <c r="D83" s="24"/>
+      <c r="C83" s="24">
+        <v>0.47</v>
+      </c>
+      <c r="D83" s="24">
+        <v>0.47</v>
+      </c>
     </row>
     <row r="84" spans="1:6">
       <c r="B84" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
+      <c r="C84" s="24">
+        <v>0.35</v>
+      </c>
+      <c r="D84" s="24">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="85" spans="1:6">
       <c r="B85" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
+      <c r="C85" s="24">
+        <v>0.02</v>
+      </c>
+      <c r="D85" s="24">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="95" spans="1:6" customHeight="1" ht="15"/>
     <row r="96" spans="1:6">
@@ -1326,158 +1405,218 @@
         <v>30</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E96" s="27" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="B97" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C97" s="29"/>
-      <c r="D97" s="29"/>
-      <c r="E97" s="30"/>
+        <v>33</v>
+      </c>
+      <c r="C97" s="29">
+        <v>0.42</v>
+      </c>
+      <c r="D97" s="29">
+        <v>0.47</v>
+      </c>
+      <c r="E97" s="30">
+        <v>0.47</v>
+      </c>
     </row>
     <row r="98" spans="1:6">
       <c r="B98" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C98" s="29"/>
-      <c r="D98" s="29"/>
-      <c r="E98" s="30"/>
+        <v>34</v>
+      </c>
+      <c r="C98" s="29">
+        <v>0.3</v>
+      </c>
+      <c r="D98" s="29">
+        <v>0.35</v>
+      </c>
+      <c r="E98" s="30">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="99" spans="1:6" customHeight="1" ht="15">
       <c r="B99" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C99" s="32"/>
-      <c r="D99" s="32"/>
-      <c r="E99" s="33"/>
+        <v>35</v>
+      </c>
+      <c r="C99" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="D99" s="32">
+        <v>0.01</v>
+      </c>
+      <c r="E99" s="33">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="108" spans="1:6" customHeight="1" ht="15"/>
     <row r="109" spans="1:6">
       <c r="B109" s="25"/>
       <c r="C109" s="26" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D109" s="26" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E109" s="27" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="B110" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C110" s="29"/>
-      <c r="D110" s="29"/>
-      <c r="E110" s="30"/>
+        <v>32</v>
+      </c>
+      <c r="C110" s="29">
+        <v>5.62</v>
+      </c>
+      <c r="D110" s="29">
+        <v>65.75</v>
+      </c>
+      <c r="E110" s="30">
+        <v>24.56</v>
+      </c>
     </row>
     <row r="111" spans="1:6">
       <c r="B111" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C111" s="29"/>
-      <c r="D111" s="29"/>
-      <c r="E111" s="30"/>
+        <v>31</v>
+      </c>
+      <c r="C111" s="29">
+        <v>5.38</v>
+      </c>
+      <c r="D111" s="29">
+        <v>57.51</v>
+      </c>
+      <c r="E111" s="30">
+        <v>24.34</v>
+      </c>
     </row>
     <row r="112" spans="1:6">
       <c r="B112" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C112" s="29"/>
-      <c r="D112" s="29"/>
-      <c r="E112" s="30"/>
+        <v>30</v>
+      </c>
+      <c r="C112" s="29">
+        <v>5.12</v>
+      </c>
+      <c r="D112" s="29">
+        <v>85.04</v>
+      </c>
+      <c r="E112" s="30">
+        <v>75.7</v>
+      </c>
     </row>
     <row r="113" spans="1:6">
       <c r="B113" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C113" s="29"/>
-      <c r="D113" s="29"/>
-      <c r="E113" s="30"/>
+        <v>39</v>
+      </c>
+      <c r="C113" s="29">
+        <v>3.88</v>
+      </c>
+      <c r="D113" s="29">
+        <v>109.13</v>
+      </c>
+      <c r="E113" s="30">
+        <v>59.35</v>
+      </c>
     </row>
     <row r="114" spans="1:6" customHeight="1" ht="15">
       <c r="B114" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C114" s="32"/>
-      <c r="D114" s="32"/>
-      <c r="E114" s="30"/>
+        <v>40</v>
+      </c>
+      <c r="C114" s="32">
+        <v>0.005</v>
+      </c>
+      <c r="D114" s="32">
+        <v>68.18</v>
+      </c>
+      <c r="E114" s="30">
+        <v>21.39</v>
+      </c>
     </row>
     <row r="115" spans="1:6" customHeight="1" ht="15">
       <c r="B115" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C115" s="32"/>
-      <c r="D115" s="32"/>
-      <c r="E115" s="33"/>
+        <v>41</v>
+      </c>
+      <c r="C115" s="32">
+        <v>0</v>
+      </c>
+      <c r="D115" s="32">
+        <v>0</v>
+      </c>
+      <c r="E115" s="33">
+        <v>18.42</v>
+      </c>
     </row>
     <row r="122" spans="1:6">
       <c r="C122" s="29" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D122" s="29" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="C123" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D123" s="34"/>
+        <v>44</v>
+      </c>
+      <c r="D123" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" spans="1:6">
       <c r="C124" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D124" s="34"/>
+        <v>45</v>
+      </c>
+      <c r="D124" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="125" spans="1:6">
       <c r="C125" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D125" s="34"/>
+        <v>46</v>
+      </c>
+      <c r="D125" s="34">
+        <v>0</v>
+      </c>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="29" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="C134" s="29" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D134" s="34"/>
     </row>
     <row r="135" spans="1:6">
       <c r="C135" s="29" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D135" s="34"/>
     </row>
     <row r="136" spans="1:6">
       <c r="C136" s="29" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D136" s="34"/>
     </row>
     <row r="137" spans="1:6">
       <c r="C137" s="29" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D137" s="34"/>
     </row>
     <row r="138" spans="1:6">
       <c r="C138" s="29" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D138" s="34"/>
     </row>
@@ -1489,7 +1628,7 @@
     </row>
     <row r="154" spans="1:6">
       <c r="B154" s="35" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C154" s="29"/>
       <c r="D154" s="29"/>
@@ -1497,7 +1636,7 @@
     </row>
     <row r="155" spans="1:6">
       <c r="B155" s="35" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C155" s="29"/>
       <c r="D155" s="29"/>
@@ -1505,7 +1644,7 @@
     </row>
     <row r="156" spans="1:6">
       <c r="B156" s="35" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C156" s="29"/>
       <c r="D156" s="29"/>
@@ -1513,7 +1652,7 @@
     </row>
     <row r="157" spans="1:6">
       <c r="B157" s="35" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C157" s="29"/>
       <c r="D157" s="29"/>
@@ -1521,21 +1660,21 @@
     </row>
     <row r="483" spans="1:6" customHeight="1" ht="28">
       <c r="B483" s="36" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C483" s="37" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D483" s="37" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E483" s="37" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="484" spans="1:6">
       <c r="B484" s="29" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C484" s="38"/>
       <c r="D484" s="38"/>
@@ -1543,7 +1682,7 @@
     </row>
     <row r="485" spans="1:6">
       <c r="B485" s="29" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C485" s="38"/>
       <c r="D485" s="38"/>
@@ -1551,7 +1690,7 @@
     </row>
     <row r="493" spans="1:6">
       <c r="C493" s="51" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D493" s="52"/>
       <c r="E493" s="50"/>
@@ -1559,7 +1698,7 @@
     </row>
     <row r="494" spans="1:6">
       <c r="C494" s="51" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D494" s="52"/>
       <c r="E494" s="50"/>
@@ -1567,7 +1706,7 @@
     </row>
     <row r="495" spans="1:6">
       <c r="C495" s="51" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D495" s="52"/>
       <c r="E495" s="50"/>
@@ -1575,7 +1714,7 @@
     </row>
     <row r="496" spans="1:6">
       <c r="C496" s="51" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D496" s="52"/>
       <c r="E496" s="50"/>
@@ -1625,7 +1764,7 @@
     </row>
     <row r="504" spans="1:6">
       <c r="C504" s="51" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D504" s="52"/>
       <c r="E504" s="50"/>
@@ -1633,7 +1772,7 @@
     </row>
     <row r="505" spans="1:6">
       <c r="C505" s="51" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D505" s="52"/>
       <c r="E505" s="50"/>
@@ -1641,7 +1780,7 @@
     </row>
     <row r="506" spans="1:6">
       <c r="C506" s="51" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D506" s="52"/>
       <c r="E506" s="50"/>
@@ -1649,7 +1788,7 @@
     </row>
     <row r="507" spans="1:6">
       <c r="C507" s="51" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D507" s="52"/>
       <c r="E507" s="50"/>
@@ -1699,19 +1838,19 @@
     </row>
     <row r="515" spans="1:6">
       <c r="C515" s="29" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D515" s="29" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="E515" s="29" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="F515" s="50"/>
     </row>
     <row r="516" spans="1:6">
       <c r="C516" s="29" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D516" s="53"/>
       <c r="E516" s="54"/>
@@ -1719,7 +1858,7 @@
     </row>
     <row r="517" spans="1:6">
       <c r="C517" s="29" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D517" s="53"/>
       <c r="E517" s="54"/>
@@ -1727,7 +1866,7 @@
     </row>
     <row r="518" spans="1:6">
       <c r="C518" s="29" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D518" s="53"/>
       <c r="E518" s="54"/>
@@ -1737,18 +1876,18 @@
     <row r="531" spans="1:6">
       <c r="B531" s="25"/>
       <c r="C531" s="26" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D531" s="26" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E531" s="27" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="532" spans="1:6">
       <c r="B532" s="28" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C532" s="29"/>
       <c r="D532" s="29"/>
@@ -1756,7 +1895,7 @@
     </row>
     <row r="533" spans="1:6">
       <c r="B533" s="28" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C533" s="29"/>
       <c r="D533" s="29"/>
@@ -1764,7 +1903,7 @@
     </row>
     <row r="534" spans="1:6">
       <c r="B534" s="28" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C534" s="29"/>
       <c r="D534" s="29"/>
@@ -1772,7 +1911,7 @@
     </row>
     <row r="535" spans="1:6">
       <c r="B535" s="28" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C535" s="29"/>
       <c r="D535" s="29"/>
@@ -1780,7 +1919,7 @@
     </row>
     <row r="536" spans="1:6" customHeight="1" ht="15">
       <c r="B536" s="28" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C536" s="32"/>
       <c r="D536" s="32"/>
@@ -1788,7 +1927,7 @@
     </row>
     <row r="537" spans="1:6" customHeight="1" ht="15">
       <c r="B537" s="31" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C537" s="32"/>
       <c r="D537" s="32"/>

</xml_diff>

<commit_message>
input sheet burn with company name
</commit_message>
<xml_diff>
--- a/phpdocx/template/graph_excel.xlsx
+++ b/phpdocx/template/graph_excel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>Shareholding Pattern</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Non-Executive</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>Non-Promoter</t>
@@ -980,86 +977,46 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4" s="2"/>
-      <c r="C4" s="3">
-        <v>2015</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2014</v>
-      </c>
-      <c r="E4" s="3">
-        <v>2013</v>
-      </c>
-      <c r="F4" s="3">
-        <v>2012</v>
-      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
-        <v>37.96</v>
-      </c>
-      <c r="D6" s="5">
-        <v>42.1</v>
-      </c>
-      <c r="E6" s="5">
-        <v>40.52</v>
-      </c>
-      <c r="F6" s="5">
-        <v>39.02</v>
-      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="5">
-        <v>15.1</v>
-      </c>
-      <c r="D7" s="5">
-        <v>-42.1</v>
-      </c>
-      <c r="E7" s="5">
-        <v>17.51</v>
-      </c>
-      <c r="F7" s="5">
-        <v>16.57</v>
-      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5">
-        <v>46.94</v>
-      </c>
-      <c r="D8" s="5">
-        <v>100</v>
-      </c>
-      <c r="E8" s="5">
-        <v>41.97</v>
-      </c>
-      <c r="F8" s="5">
-        <v>44.41</v>
-      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="6" t="s">
@@ -1071,25 +1028,19 @@
       <c r="B16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="8">
-        <v>2</v>
-      </c>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:6">
       <c r="B17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="8">
-        <v>0</v>
-      </c>
+      <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="8">
-        <v>8</v>
-      </c>
+      <c r="C18" s="8"/>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" s="46"/>
@@ -1105,10 +1056,10 @@
         <v>10</v>
       </c>
       <c r="C28" s="49">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="D28" s="49">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1116,10 +1067,10 @@
         <v>11</v>
       </c>
       <c r="C29" s="49">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="D29" s="49">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1147,59 +1098,29 @@
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="B38" s="12">
-        <v>2011</v>
-      </c>
-      <c r="C38" s="19">
-        <v>0</v>
-      </c>
-      <c r="D38" s="13">
-        <v>125.66</v>
-      </c>
+      <c r="B38" s="12"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="13"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="B39" s="12">
-        <v>2012</v>
-      </c>
-      <c r="C39" s="19">
-        <v>0</v>
-      </c>
-      <c r="D39" s="13">
-        <v>115.26</v>
-      </c>
+      <c r="B39" s="12"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="13"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="B40" s="12">
-        <v>2013</v>
-      </c>
-      <c r="C40" s="19">
-        <v>0</v>
-      </c>
-      <c r="D40" s="13">
-        <v>119.33</v>
-      </c>
+      <c r="B40" s="12"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="13"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="B41" s="12">
-        <v>2014</v>
-      </c>
-      <c r="C41" s="19">
-        <v>0.83</v>
-      </c>
-      <c r="D41" s="13">
-        <v>138.61</v>
-      </c>
+      <c r="B41" s="12"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="13"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="B42" s="14">
-        <v>2015</v>
-      </c>
-      <c r="C42" s="20">
-        <v>6.08</v>
-      </c>
-      <c r="D42" s="15">
-        <v>186.28</v>
-      </c>
+      <c r="B42" s="14"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="15"/>
     </row>
     <row r="48" spans="1:6">
       <c r="B48" t="s">
@@ -1219,34 +1140,26 @@
       <c r="B50" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>19</v>
-      </c>
+      <c r="C50" s="17"/>
+      <c r="D50" s="18"/>
     </row>
     <row r="51" spans="1:6">
       <c r="B51" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C51" s="17">
-        <v>5.32</v>
-      </c>
-      <c r="D51" s="18">
-        <v>0.87</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C51" s="17"/>
+      <c r="D51" s="18"/>
     </row>
     <row r="59" spans="1:6">
       <c r="B59" s="39"/>
       <c r="C59" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D59" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="D59" s="40" t="s">
+      <c r="E59" s="40" t="s">
         <v>22</v>
-      </c>
-      <c r="E59" s="40" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1269,13 +1182,13 @@
     </row>
     <row r="71" spans="1:6">
       <c r="B71" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C71" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C71" s="40" t="s">
+      <c r="D71" s="40" t="s">
         <v>25</v>
-      </c>
-      <c r="D71" s="40" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1300,21 +1213,21 @@
     </row>
     <row r="83" spans="1:6">
       <c r="B83" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C83" s="24"/>
       <c r="D83" s="24"/>
     </row>
     <row r="84" spans="1:6">
       <c r="B84" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C84" s="24"/>
       <c r="D84" s="24"/>
     </row>
     <row r="85" spans="1:6">
       <c r="B85" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C85" s="24"/>
       <c r="D85" s="24"/>
@@ -1323,18 +1236,18 @@
     <row r="96" spans="1:6">
       <c r="B96" s="25"/>
       <c r="C96" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E96" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="B97" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C97" s="29"/>
       <c r="D97" s="29"/>
@@ -1342,7 +1255,7 @@
     </row>
     <row r="98" spans="1:6">
       <c r="B98" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C98" s="29"/>
       <c r="D98" s="29"/>
@@ -1350,7 +1263,7 @@
     </row>
     <row r="99" spans="1:6" customHeight="1" ht="15">
       <c r="B99" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C99" s="32"/>
       <c r="D99" s="32"/>
@@ -1360,18 +1273,18 @@
     <row r="109" spans="1:6">
       <c r="B109" s="25"/>
       <c r="C109" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D109" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D109" s="26" t="s">
+      <c r="E109" s="27" t="s">
         <v>35</v>
-      </c>
-      <c r="E109" s="27" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="B110" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C110" s="29"/>
       <c r="D110" s="29"/>
@@ -1379,7 +1292,7 @@
     </row>
     <row r="111" spans="1:6">
       <c r="B111" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C111" s="29"/>
       <c r="D111" s="29"/>
@@ -1387,7 +1300,7 @@
     </row>
     <row r="112" spans="1:6">
       <c r="B112" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C112" s="29"/>
       <c r="D112" s="29"/>
@@ -1395,7 +1308,7 @@
     </row>
     <row r="113" spans="1:6">
       <c r="B113" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C113" s="29"/>
       <c r="D113" s="29"/>
@@ -1403,7 +1316,7 @@
     </row>
     <row r="114" spans="1:6" customHeight="1" ht="15">
       <c r="B114" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C114" s="32"/>
       <c r="D114" s="32"/>
@@ -1411,7 +1324,7 @@
     </row>
     <row r="115" spans="1:6" customHeight="1" ht="15">
       <c r="B115" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C115" s="32"/>
       <c r="D115" s="32"/>
@@ -1419,65 +1332,65 @@
     </row>
     <row r="122" spans="1:6">
       <c r="C122" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D122" s="29" t="s">
         <v>38</v>
-      </c>
-      <c r="D122" s="29" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="C123" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D123" s="34"/>
     </row>
     <row r="124" spans="1:6">
       <c r="C124" s="29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D124" s="34"/>
     </row>
     <row r="125" spans="1:6">
       <c r="C125" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D125" s="34"/>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="C134" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D134" s="34"/>
     </row>
     <row r="135" spans="1:6">
       <c r="C135" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D135" s="34"/>
     </row>
     <row r="136" spans="1:6">
       <c r="C136" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D136" s="34"/>
     </row>
     <row r="137" spans="1:6">
       <c r="C137" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D137" s="34"/>
     </row>
     <row r="138" spans="1:6">
       <c r="C138" s="29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D138" s="34"/>
     </row>
@@ -1489,7 +1402,7 @@
     </row>
     <row r="154" spans="1:6">
       <c r="B154" s="35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C154" s="29"/>
       <c r="D154" s="29"/>
@@ -1497,7 +1410,7 @@
     </row>
     <row r="155" spans="1:6">
       <c r="B155" s="35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C155" s="29"/>
       <c r="D155" s="29"/>
@@ -1505,7 +1418,7 @@
     </row>
     <row r="156" spans="1:6">
       <c r="B156" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C156" s="29"/>
       <c r="D156" s="29"/>
@@ -1513,7 +1426,7 @@
     </row>
     <row r="157" spans="1:6">
       <c r="B157" s="35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C157" s="29"/>
       <c r="D157" s="29"/>
@@ -1521,21 +1434,21 @@
     </row>
     <row r="483" spans="1:6" customHeight="1" ht="28">
       <c r="B483" s="36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C483" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D483" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="D483" s="37" t="s">
+      <c r="E483" s="37" t="s">
         <v>49</v>
-      </c>
-      <c r="E483" s="37" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="484" spans="1:6">
       <c r="B484" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C484" s="38"/>
       <c r="D484" s="38"/>
@@ -1543,7 +1456,7 @@
     </row>
     <row r="485" spans="1:6">
       <c r="B485" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C485" s="38"/>
       <c r="D485" s="38"/>
@@ -1551,7 +1464,7 @@
     </row>
     <row r="493" spans="1:6">
       <c r="C493" s="51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D493" s="52"/>
       <c r="E493" s="50"/>
@@ -1559,7 +1472,7 @@
     </row>
     <row r="494" spans="1:6">
       <c r="C494" s="51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D494" s="52"/>
       <c r="E494" s="50"/>
@@ -1567,7 +1480,7 @@
     </row>
     <row r="495" spans="1:6">
       <c r="C495" s="51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D495" s="52"/>
       <c r="E495" s="50"/>
@@ -1575,7 +1488,7 @@
     </row>
     <row r="496" spans="1:6">
       <c r="C496" s="51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D496" s="52"/>
       <c r="E496" s="50"/>
@@ -1625,7 +1538,7 @@
     </row>
     <row r="504" spans="1:6">
       <c r="C504" s="51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D504" s="52"/>
       <c r="E504" s="50"/>
@@ -1633,7 +1546,7 @@
     </row>
     <row r="505" spans="1:6">
       <c r="C505" s="51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D505" s="52"/>
       <c r="E505" s="50"/>
@@ -1641,7 +1554,7 @@
     </row>
     <row r="506" spans="1:6">
       <c r="C506" s="51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D506" s="52"/>
       <c r="E506" s="50"/>
@@ -1649,7 +1562,7 @@
     </row>
     <row r="507" spans="1:6">
       <c r="C507" s="51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D507" s="52"/>
       <c r="E507" s="50"/>
@@ -1699,19 +1612,19 @@
     </row>
     <row r="515" spans="1:6">
       <c r="C515" s="29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D515" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E515" s="29" t="s">
         <v>52</v>
-      </c>
-      <c r="E515" s="29" t="s">
-        <v>53</v>
       </c>
       <c r="F515" s="50"/>
     </row>
     <row r="516" spans="1:6">
       <c r="C516" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D516" s="53"/>
       <c r="E516" s="54"/>
@@ -1719,7 +1632,7 @@
     </row>
     <row r="517" spans="1:6">
       <c r="C517" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D517" s="53"/>
       <c r="E517" s="54"/>
@@ -1727,7 +1640,7 @@
     </row>
     <row r="518" spans="1:6">
       <c r="C518" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D518" s="53"/>
       <c r="E518" s="54"/>
@@ -1737,18 +1650,18 @@
     <row r="531" spans="1:6">
       <c r="B531" s="25"/>
       <c r="C531" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D531" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D531" s="26" t="s">
+      <c r="E531" s="27" t="s">
         <v>35</v>
-      </c>
-      <c r="E531" s="27" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="532" spans="1:6">
       <c r="B532" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C532" s="29"/>
       <c r="D532" s="29"/>
@@ -1756,7 +1669,7 @@
     </row>
     <row r="533" spans="1:6">
       <c r="B533" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C533" s="29"/>
       <c r="D533" s="29"/>
@@ -1764,7 +1677,7 @@
     </row>
     <row r="534" spans="1:6">
       <c r="B534" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C534" s="29"/>
       <c r="D534" s="29"/>
@@ -1772,7 +1685,7 @@
     </row>
     <row r="535" spans="1:6">
       <c r="B535" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C535" s="29"/>
       <c r="D535" s="29"/>
@@ -1780,7 +1693,7 @@
     </row>
     <row r="536" spans="1:6" customHeight="1" ht="15">
       <c r="B536" s="28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C536" s="32"/>
       <c r="D536" s="32"/>
@@ -1788,7 +1701,7 @@
     </row>
     <row r="537" spans="1:6" customHeight="1" ht="15">
       <c r="B537" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C537" s="32"/>
       <c r="D537" s="32"/>

</xml_diff>

<commit_message>
Burning issues and delete directors
</commit_message>
<xml_diff>
--- a/phpdocx/template/graph_excel.xlsx
+++ b/phpdocx/template/graph_excel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="58">
   <si>
     <t>Shareholding Pattern</t>
   </si>
@@ -74,6 +74,9 @@
     <t>Non-Executive</t>
   </si>
   <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>Non-Promoter</t>
   </si>
   <si>
@@ -104,76 +107,88 @@
     <t>Non Audit</t>
   </si>
   <si>
+    <t>FY 12/13</t>
+  </si>
+  <si>
+    <t>FY 13/14</t>
+  </si>
+  <si>
+    <t>FY 14/15</t>
+  </si>
+  <si>
+    <t>Audit Fee</t>
+  </si>
+  <si>
+    <t>Audit Related Fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non Audit Fee </t>
+  </si>
+  <si>
+    <t>ED Remuneration</t>
+  </si>
+  <si>
+    <t>Indexed TSR</t>
+  </si>
+  <si>
+    <t>Net Profit</t>
+  </si>
+  <si>
+    <t>FY -1/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Commission</t>
+  </si>
+  <si>
+    <t>Promoter NED</t>
+  </si>
+  <si>
+    <t>Independent Directors</t>
+  </si>
+  <si>
+    <t>Other NEDs</t>
+  </si>
+  <si>
+    <t>Total Commission</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>1Y</t>
+  </si>
+  <si>
+    <t>3Y</t>
+  </si>
+  <si>
+    <t>5Y</t>
+  </si>
+  <si>
+    <t>Existing Borrowing</t>
+  </si>
+  <si>
+    <t>Unavailed borrowing limit</t>
+  </si>
+  <si>
+    <t>Proposed increase</t>
+  </si>
+  <si>
+    <t>'</t>
+  </si>
+  <si>
+    <t>CSR</t>
+  </si>
+  <si>
+    <t>CSR as % of Net Profit</t>
+  </si>
+  <si>
     <t>FY -1/0</t>
   </si>
   <si>
-    <t>Audit Fee</t>
-  </si>
-  <si>
-    <t>Audit Related Fee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non Audit Fee </t>
-  </si>
-  <si>
-    <t>ED Remuneration</t>
-  </si>
-  <si>
-    <t>Indexed TSR</t>
-  </si>
-  <si>
-    <t>Net Profit</t>
-  </si>
-  <si>
-    <t>FY -1/</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Commission</t>
-  </si>
-  <si>
-    <t>Promoter NED</t>
-  </si>
-  <si>
-    <t>Independent Directors</t>
-  </si>
-  <si>
-    <t>Other NEDs</t>
-  </si>
-  <si>
-    <t>Total Commission</t>
-  </si>
-  <si>
-    <t>Today</t>
-  </si>
-  <si>
-    <t>1Y</t>
-  </si>
-  <si>
-    <t>3Y</t>
-  </si>
-  <si>
-    <t>5Y</t>
-  </si>
-  <si>
-    <t>Existing Borrowing</t>
-  </si>
-  <si>
-    <t>Unavailed borrowing limit</t>
-  </si>
-  <si>
-    <t>Proposed increase</t>
-  </si>
-  <si>
-    <t>'</t>
-  </si>
-  <si>
-    <t>CSR</t>
-  </si>
-  <si>
-    <t>CSR as % of Net Profit</t>
+    <t>FY -1/00</t>
   </si>
 </sst>
 </file>
@@ -977,46 +992,86 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="C4" s="3">
+        <v>2015</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2014</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2013</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2012</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="C5" s="5">
+        <v>43.66</v>
+      </c>
+      <c r="D5" s="5">
+        <v>42.17</v>
+      </c>
+      <c r="E5" s="5">
+        <v>42.23</v>
+      </c>
+      <c r="F5" s="5">
+        <v>42.1</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="C6" s="5">
+        <v>20.42</v>
+      </c>
+      <c r="D6" s="5">
+        <v>22.53</v>
+      </c>
+      <c r="E6" s="5">
+        <v>20.81</v>
+      </c>
+      <c r="F6" s="5">
+        <v>14.08</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="C7" s="5">
+        <v>14.48</v>
+      </c>
+      <c r="D7" s="5">
+        <v>11.26</v>
+      </c>
+      <c r="E7" s="5">
+        <v>11.89</v>
+      </c>
+      <c r="F7" s="5">
+        <v>16.16</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="C8" s="5">
+        <v>21.44</v>
+      </c>
+      <c r="D8" s="5">
+        <v>24.04</v>
+      </c>
+      <c r="E8" s="5">
+        <v>25.07</v>
+      </c>
+      <c r="F8" s="5">
+        <v>27.66</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="6" t="s">
@@ -1028,19 +1083,25 @@
       <c r="B16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="8"/>
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="B17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="8">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" spans="1:6">
       <c r="B27" s="46"/>
@@ -1056,10 +1117,10 @@
         <v>10</v>
       </c>
       <c r="C28" s="49">
-        <v>0</v>
+        <v>0.63</v>
       </c>
       <c r="D28" s="49">
-        <v>0</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1067,10 +1128,10 @@
         <v>11</v>
       </c>
       <c r="C29" s="49">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="D29" s="49">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1098,29 +1159,59 @@
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="B38" s="12"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="13"/>
+      <c r="B38" s="12">
+        <v>2011</v>
+      </c>
+      <c r="C38" s="19">
+        <v>1.0954</v>
+      </c>
+      <c r="D38" s="13">
+        <v>136.9</v>
+      </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="B39" s="12"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="13"/>
+      <c r="B39" s="12">
+        <v>2012</v>
+      </c>
+      <c r="C39" s="19">
+        <v>1.3471</v>
+      </c>
+      <c r="D39" s="13">
+        <v>187.36</v>
+      </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="B40" s="12"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="13"/>
+      <c r="B40" s="12">
+        <v>2013</v>
+      </c>
+      <c r="C40" s="19">
+        <v>1.6936</v>
+      </c>
+      <c r="D40" s="13">
+        <v>143.49</v>
+      </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="B41" s="12"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="13"/>
+      <c r="B41" s="12">
+        <v>2014</v>
+      </c>
+      <c r="C41" s="19">
+        <v>1.6386</v>
+      </c>
+      <c r="D41" s="13">
+        <v>178.48</v>
+      </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="B42" s="14"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="15"/>
+      <c r="B42" s="14">
+        <v>2015</v>
+      </c>
+      <c r="C42" s="20">
+        <v>1.546</v>
+      </c>
+      <c r="D42" s="15">
+        <v>225.53</v>
+      </c>
     </row>
     <row r="48" spans="1:6">
       <c r="B48" t="s">
@@ -1140,151 +1231,235 @@
       <c r="B50" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="18"/>
+      <c r="C50" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="18">
+        <v>0.77</v>
+      </c>
     </row>
     <row r="51" spans="1:6">
       <c r="B51" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" s="17"/>
-      <c r="D51" s="18"/>
+        <v>20</v>
+      </c>
+      <c r="C51" s="17">
+        <v>1.55</v>
+      </c>
+      <c r="D51" s="18">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="59" spans="1:6">
       <c r="B59" s="39"/>
       <c r="C59" s="40" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D59" s="40" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E59" s="40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="B60" s="40"/>
-      <c r="C60" s="41"/>
-      <c r="D60" s="42"/>
-      <c r="E60" s="43"/>
+      <c r="B60" s="40">
+        <v>2013</v>
+      </c>
+      <c r="C60" s="41">
+        <v>1.25</v>
+      </c>
+      <c r="D60" s="42">
+        <v>3.98</v>
+      </c>
+      <c r="E60" s="43">
+        <v>0.37</v>
+      </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="B61" s="40"/>
-      <c r="C61" s="41"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="43"/>
+      <c r="B61" s="40">
+        <v>2014</v>
+      </c>
+      <c r="C61" s="41">
+        <v>1.25</v>
+      </c>
+      <c r="D61" s="42">
+        <v>3.88</v>
+      </c>
+      <c r="E61" s="43">
+        <v>0.37</v>
+      </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="B62" s="40"/>
-      <c r="C62" s="41"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="43"/>
+      <c r="B62" s="40">
+        <v>2015</v>
+      </c>
+      <c r="C62" s="41">
+        <v>1.25</v>
+      </c>
+      <c r="D62" s="42">
+        <v>7.89</v>
+      </c>
+      <c r="E62" s="43">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="71" spans="1:6">
       <c r="B71" s="40" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C71" s="40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D71" s="40" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="B72" s="41"/>
-      <c r="C72" s="41"/>
-      <c r="D72" s="43"/>
+      <c r="B72" s="41">
+        <v>1.25</v>
+      </c>
+      <c r="C72" s="41">
+        <v>7.89</v>
+      </c>
+      <c r="D72" s="43">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="B73" s="41"/>
-      <c r="C73" s="41"/>
-      <c r="D73" s="43"/>
+      <c r="B73" s="41">
+        <v>5</v>
+      </c>
+      <c r="C73" s="41">
+        <v>18.25</v>
+      </c>
+      <c r="D73" s="43">
+        <v>0.32</v>
+      </c>
     </row>
     <row r="74" spans="1:6">
-      <c r="B74" s="41"/>
-      <c r="C74" s="41"/>
-      <c r="D74" s="43"/>
+      <c r="B74" s="41">
+        <v>59.5</v>
+      </c>
+      <c r="C74" s="41">
+        <v>105.91</v>
+      </c>
+      <c r="D74" s="43">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="82" spans="1:6">
       <c r="B82" s="21"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="22"/>
+      <c r="C82" s="22">
+        <v>2015</v>
+      </c>
+      <c r="D82" s="22">
+        <v>2014</v>
+      </c>
     </row>
     <row r="83" spans="1:6">
       <c r="B83" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C83" s="24"/>
-      <c r="D83" s="24"/>
+        <v>27</v>
+      </c>
+      <c r="C83" s="24">
+        <v>50</v>
+      </c>
+      <c r="D83" s="24">
+        <v>0.225</v>
+      </c>
     </row>
     <row r="84" spans="1:6">
       <c r="B84" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
+        <v>28</v>
+      </c>
+      <c r="C84" s="24">
+        <v>0.06</v>
+      </c>
+      <c r="D84" s="24">
+        <v>54.25</v>
+      </c>
     </row>
     <row r="85" spans="1:6">
       <c r="B85" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
+        <v>29</v>
+      </c>
+      <c r="C85" s="24">
+        <v>0.285</v>
+      </c>
+      <c r="D85" s="24">
+        <v>0.338</v>
+      </c>
     </row>
     <row r="95" spans="1:6" customHeight="1" ht="15"/>
     <row r="96" spans="1:6">
       <c r="B96" s="25"/>
       <c r="C96" s="26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E96" s="27" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="B97" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C97" s="29"/>
-      <c r="D97" s="29"/>
-      <c r="E97" s="30"/>
+        <v>33</v>
+      </c>
+      <c r="C97" s="29">
+        <v>0.225</v>
+      </c>
+      <c r="D97" s="29">
+        <v>0.225</v>
+      </c>
+      <c r="E97" s="30">
+        <v>50</v>
+      </c>
     </row>
     <row r="98" spans="1:6">
       <c r="B98" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C98" s="29"/>
-      <c r="D98" s="29"/>
-      <c r="E98" s="30"/>
+        <v>34</v>
+      </c>
+      <c r="C98" s="29">
+        <v>0.04</v>
+      </c>
+      <c r="D98" s="29">
+        <v>54.25</v>
+      </c>
+      <c r="E98" s="30">
+        <v>0.06</v>
+      </c>
     </row>
     <row r="99" spans="1:6" customHeight="1" ht="15">
       <c r="B99" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C99" s="32"/>
-      <c r="D99" s="32"/>
-      <c r="E99" s="33"/>
+        <v>35</v>
+      </c>
+      <c r="C99" s="32">
+        <v>37.35</v>
+      </c>
+      <c r="D99" s="32">
+        <v>0.338</v>
+      </c>
+      <c r="E99" s="33">
+        <v>0.285</v>
+      </c>
     </row>
     <row r="108" spans="1:6" customHeight="1" ht="15"/>
     <row r="109" spans="1:6">
       <c r="B109" s="25"/>
       <c r="C109" s="26" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D109" s="26" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E109" s="27" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="B110" s="28" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C110" s="29"/>
       <c r="D110" s="29"/>
@@ -1292,7 +1467,7 @@
     </row>
     <row r="111" spans="1:6">
       <c r="B111" s="28" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C111" s="29"/>
       <c r="D111" s="29"/>
@@ -1300,7 +1475,7 @@
     </row>
     <row r="112" spans="1:6">
       <c r="B112" s="28" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C112" s="29"/>
       <c r="D112" s="29"/>
@@ -1308,7 +1483,7 @@
     </row>
     <row r="113" spans="1:6">
       <c r="B113" s="28" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C113" s="29"/>
       <c r="D113" s="29"/>
@@ -1316,7 +1491,7 @@
     </row>
     <row r="114" spans="1:6" customHeight="1" ht="15">
       <c r="B114" s="28" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C114" s="32"/>
       <c r="D114" s="32"/>
@@ -1324,7 +1499,7 @@
     </row>
     <row r="115" spans="1:6" customHeight="1" ht="15">
       <c r="B115" s="31" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C115" s="32"/>
       <c r="D115" s="32"/>
@@ -1332,65 +1507,65 @@
     </row>
     <row r="122" spans="1:6">
       <c r="C122" s="29" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D122" s="29" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="C123" s="29" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D123" s="34"/>
     </row>
     <row r="124" spans="1:6">
       <c r="C124" s="29" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D124" s="34"/>
     </row>
     <row r="125" spans="1:6">
       <c r="C125" s="29" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D125" s="34"/>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="29" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D133" s="29" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="C134" s="29" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D134" s="34"/>
     </row>
     <row r="135" spans="1:6">
       <c r="C135" s="29" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D135" s="34"/>
     </row>
     <row r="136" spans="1:6">
       <c r="C136" s="29" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D136" s="34"/>
     </row>
     <row r="137" spans="1:6">
       <c r="C137" s="29" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D137" s="34"/>
     </row>
     <row r="138" spans="1:6">
       <c r="C138" s="29" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D138" s="34"/>
     </row>
@@ -1402,7 +1577,7 @@
     </row>
     <row r="154" spans="1:6">
       <c r="B154" s="35" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C154" s="29"/>
       <c r="D154" s="29"/>
@@ -1410,7 +1585,7 @@
     </row>
     <row r="155" spans="1:6">
       <c r="B155" s="35" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C155" s="29"/>
       <c r="D155" s="29"/>
@@ -1418,7 +1593,7 @@
     </row>
     <row r="156" spans="1:6">
       <c r="B156" s="35" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C156" s="29"/>
       <c r="D156" s="29"/>
@@ -1426,7 +1601,7 @@
     </row>
     <row r="157" spans="1:6">
       <c r="B157" s="35" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C157" s="29"/>
       <c r="D157" s="29"/>
@@ -1434,21 +1609,21 @@
     </row>
     <row r="483" spans="1:6" customHeight="1" ht="28">
       <c r="B483" s="36" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C483" s="37" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D483" s="37" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E483" s="37" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="484" spans="1:6">
       <c r="B484" s="29" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C484" s="38"/>
       <c r="D484" s="38"/>
@@ -1456,7 +1631,7 @@
     </row>
     <row r="485" spans="1:6">
       <c r="B485" s="29" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C485" s="38"/>
       <c r="D485" s="38"/>
@@ -1464,7 +1639,7 @@
     </row>
     <row r="493" spans="1:6">
       <c r="C493" s="51" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D493" s="52"/>
       <c r="E493" s="50"/>
@@ -1472,7 +1647,7 @@
     </row>
     <row r="494" spans="1:6">
       <c r="C494" s="51" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D494" s="52"/>
       <c r="E494" s="50"/>
@@ -1480,7 +1655,7 @@
     </row>
     <row r="495" spans="1:6">
       <c r="C495" s="51" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D495" s="52"/>
       <c r="E495" s="50"/>
@@ -1488,7 +1663,7 @@
     </row>
     <row r="496" spans="1:6">
       <c r="C496" s="51" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D496" s="52"/>
       <c r="E496" s="50"/>
@@ -1538,7 +1713,7 @@
     </row>
     <row r="504" spans="1:6">
       <c r="C504" s="51" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D504" s="52"/>
       <c r="E504" s="50"/>
@@ -1546,7 +1721,7 @@
     </row>
     <row r="505" spans="1:6">
       <c r="C505" s="51" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D505" s="52"/>
       <c r="E505" s="50"/>
@@ -1554,7 +1729,7 @@
     </row>
     <row r="506" spans="1:6">
       <c r="C506" s="51" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D506" s="52"/>
       <c r="E506" s="50"/>
@@ -1562,7 +1737,7 @@
     </row>
     <row r="507" spans="1:6">
       <c r="C507" s="51" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D507" s="52"/>
       <c r="E507" s="50"/>
@@ -1612,19 +1787,19 @@
     </row>
     <row r="515" spans="1:6">
       <c r="C515" s="29" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D515" s="29" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E515" s="29" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F515" s="50"/>
     </row>
     <row r="516" spans="1:6">
       <c r="C516" s="29" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D516" s="53"/>
       <c r="E516" s="54"/>
@@ -1632,7 +1807,7 @@
     </row>
     <row r="517" spans="1:6">
       <c r="C517" s="29" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D517" s="53"/>
       <c r="E517" s="54"/>
@@ -1640,7 +1815,7 @@
     </row>
     <row r="518" spans="1:6">
       <c r="C518" s="29" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="D518" s="53"/>
       <c r="E518" s="54"/>
@@ -1650,18 +1825,18 @@
     <row r="531" spans="1:6">
       <c r="B531" s="25"/>
       <c r="C531" s="26" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D531" s="26" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E531" s="27" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="532" spans="1:6">
       <c r="B532" s="28" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C532" s="29"/>
       <c r="D532" s="29"/>
@@ -1669,7 +1844,7 @@
     </row>
     <row r="533" spans="1:6">
       <c r="B533" s="28" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C533" s="29"/>
       <c r="D533" s="29"/>
@@ -1677,7 +1852,7 @@
     </row>
     <row r="534" spans="1:6">
       <c r="B534" s="28" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C534" s="29"/>
       <c r="D534" s="29"/>
@@ -1685,7 +1860,7 @@
     </row>
     <row r="535" spans="1:6">
       <c r="B535" s="28" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C535" s="29"/>
       <c r="D535" s="29"/>
@@ -1693,7 +1868,7 @@
     </row>
     <row r="536" spans="1:6" customHeight="1" ht="15">
       <c r="B536" s="28" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C536" s="32"/>
       <c r="D536" s="32"/>
@@ -1701,7 +1876,7 @@
     </row>
     <row r="537" spans="1:6" customHeight="1" ht="15">
       <c r="B537" s="31" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C537" s="32"/>
       <c r="D537" s="32"/>

</xml_diff>

<commit_message>
solved downloading issue of report id 172
</commit_message>
<xml_diff>
--- a/phpdocx/template/graph_excel.xlsx
+++ b/phpdocx/template/graph_excel.xlsx
@@ -74,10 +74,10 @@
     <t>Non-Executive</t>
   </si>
   <si>
+    <t>Non-Promoter</t>
+  </si>
+  <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>Non-Promoter</t>
   </si>
   <si>
     <t>Dividend (LHS)</t>
@@ -1010,16 +1010,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="5">
-        <v>43.66</v>
+        <v>70</v>
       </c>
       <c r="D5" s="5">
-        <v>42.17</v>
+        <v>70</v>
       </c>
       <c r="E5" s="5">
-        <v>42.23</v>
+        <v>70</v>
       </c>
       <c r="F5" s="5">
-        <v>42.1</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1027,16 +1027,16 @@
         <v>2</v>
       </c>
       <c r="C6" s="5">
-        <v>20.42</v>
+        <v>5.85</v>
       </c>
       <c r="D6" s="5">
-        <v>22.53</v>
+        <v>11.93</v>
       </c>
       <c r="E6" s="5">
-        <v>20.81</v>
+        <v>10.8</v>
       </c>
       <c r="F6" s="5">
-        <v>14.08</v>
+        <v>11.18</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1044,16 +1044,16 @@
         <v>3</v>
       </c>
       <c r="C7" s="5">
-        <v>14.48</v>
+        <v>0.01</v>
       </c>
       <c r="D7" s="5">
-        <v>11.26</v>
+        <v>0.16</v>
       </c>
       <c r="E7" s="5">
-        <v>11.89</v>
+        <v>0.16</v>
       </c>
       <c r="F7" s="5">
-        <v>16.16</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1061,16 +1061,16 @@
         <v>4</v>
       </c>
       <c r="C8" s="5">
-        <v>21.44</v>
+        <v>24.22</v>
       </c>
       <c r="D8" s="5">
-        <v>24.04</v>
+        <v>15.61</v>
       </c>
       <c r="E8" s="5">
-        <v>25.07</v>
+        <v>16.95</v>
       </c>
       <c r="F8" s="5">
-        <v>27.66</v>
+        <v>18.86</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1084,7 +1084,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1100,7 +1100,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1117,10 +1117,10 @@
         <v>10</v>
       </c>
       <c r="C28" s="49">
-        <v>0.63</v>
+        <v>0.5</v>
       </c>
       <c r="D28" s="49">
-        <v>0.38</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1128,10 +1128,10 @@
         <v>11</v>
       </c>
       <c r="C29" s="49">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D29" s="49">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1163,10 +1163,10 @@
         <v>2011</v>
       </c>
       <c r="C38" s="19">
-        <v>1.0954</v>
+        <v>0</v>
       </c>
       <c r="D38" s="13">
-        <v>136.9</v>
+        <v>92.78</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1174,10 +1174,10 @@
         <v>2012</v>
       </c>
       <c r="C39" s="19">
-        <v>1.3471</v>
+        <v>6.38</v>
       </c>
       <c r="D39" s="13">
-        <v>187.36</v>
+        <v>73.31</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1185,10 +1185,10 @@
         <v>2013</v>
       </c>
       <c r="C40" s="19">
-        <v>1.6936</v>
+        <v>6.503</v>
       </c>
       <c r="D40" s="13">
-        <v>143.49</v>
+        <v>63.78</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1196,10 +1196,10 @@
         <v>2014</v>
       </c>
       <c r="C41" s="19">
-        <v>1.6386</v>
+        <v>4.6016</v>
       </c>
       <c r="D41" s="13">
-        <v>178.48</v>
+        <v>83.6</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1207,10 +1207,10 @@
         <v>2015</v>
       </c>
       <c r="C42" s="20">
-        <v>1.546</v>
+        <v>5.2855</v>
       </c>
       <c r="D42" s="15">
-        <v>225.53</v>
+        <v>170.31</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1231,22 +1231,22 @@
       <c r="B50" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="17" t="s">
-        <v>19</v>
+      <c r="C50" s="17">
+        <v>4.24</v>
       </c>
       <c r="D50" s="18">
-        <v>0.77</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="B51" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="17">
-        <v>1.55</v>
-      </c>
       <c r="D51" s="18">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1266,13 +1266,13 @@
         <v>2013</v>
       </c>
       <c r="C60" s="41">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="D60" s="42">
-        <v>3.98</v>
+        <v>9</v>
       </c>
       <c r="E60" s="43">
-        <v>0.37</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1280,13 +1280,13 @@
         <v>2014</v>
       </c>
       <c r="C61" s="41">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="D61" s="42">
-        <v>3.88</v>
+        <v>4.5</v>
       </c>
       <c r="E61" s="43">
-        <v>0.37</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1294,13 +1294,13 @@
         <v>2015</v>
       </c>
       <c r="C62" s="41">
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="D62" s="42">
-        <v>7.89</v>
+        <v>7.7</v>
       </c>
       <c r="E62" s="43">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1316,35 +1316,35 @@
     </row>
     <row r="72" spans="1:6">
       <c r="B72" s="41">
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="C72" s="41">
-        <v>7.89</v>
+        <v>7.7</v>
       </c>
       <c r="D72" s="43">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="B73" s="41">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C73" s="41">
-        <v>18.25</v>
+        <v>7.42</v>
       </c>
       <c r="D73" s="43">
-        <v>0.32</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="B74" s="41">
-        <v>59.5</v>
+        <v>1.4</v>
       </c>
       <c r="C74" s="41">
-        <v>105.91</v>
+        <v>7.7</v>
       </c>
       <c r="D74" s="43">
-        <v>0.65</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -1361,10 +1361,10 @@
         <v>27</v>
       </c>
       <c r="C83" s="24">
-        <v>50</v>
+        <v>0.38</v>
       </c>
       <c r="D83" s="24">
-        <v>0.225</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -1372,10 +1372,10 @@
         <v>28</v>
       </c>
       <c r="C84" s="24">
-        <v>0.06</v>
+        <v>0.3</v>
       </c>
       <c r="D84" s="24">
-        <v>54.25</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -1383,10 +1383,10 @@
         <v>29</v>
       </c>
       <c r="C85" s="24">
-        <v>0.285</v>
+        <v>0.02</v>
       </c>
       <c r="D85" s="24">
-        <v>0.338</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="95" spans="1:6" customHeight="1" ht="15"/>
@@ -1407,13 +1407,13 @@
         <v>33</v>
       </c>
       <c r="C97" s="29">
-        <v>0.225</v>
+        <v>0.25</v>
       </c>
       <c r="D97" s="29">
-        <v>0.225</v>
+        <v>0.25</v>
       </c>
       <c r="E97" s="30">
-        <v>50</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -1421,13 +1421,13 @@
         <v>34</v>
       </c>
       <c r="C98" s="29">
-        <v>0.04</v>
+        <v>0.32</v>
       </c>
       <c r="D98" s="29">
-        <v>54.25</v>
+        <v>0.3</v>
       </c>
       <c r="E98" s="30">
-        <v>0.06</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="99" spans="1:6" customHeight="1" ht="15">
@@ -1435,13 +1435,13 @@
         <v>35</v>
       </c>
       <c r="C99" s="32">
-        <v>37.35</v>
+        <v>0.03</v>
       </c>
       <c r="D99" s="32">
-        <v>0.338</v>
+        <v>0.05</v>
       </c>
       <c r="E99" s="33">
-        <v>0.285</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="108" spans="1:6" customHeight="1" ht="15"/>

</xml_diff>